<commit_message>
Commit Project Progress Report for week 4.
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tuần 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tuần 2" sheetId="2" r:id="rId2"/>
     <sheet name="Tuần 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tuần 4" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuần 4'!$B$20:$G$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Tuần 4'!$A$1:$M$67</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>Task</t>
   </si>
@@ -101,13 +106,184 @@
   <si>
     <t xml:space="preserve"> Xây dựng các chức năng cần có của 1 CMS cơ bản. Thiết kế bố cục và mẫu chung cho CMS.
 </t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Thời điểm hoàn thành</t>
+  </si>
+  <si>
+    <t>Chất lượng công việc</t>
+  </si>
+  <si>
+    <t>Khối lượng CV</t>
+  </si>
+  <si>
+    <t>Chất lượng CV</t>
+  </si>
+  <si>
+    <t>Tốc độ làm việc</t>
+  </si>
+  <si>
+    <t>ĐÁNH GIÁ CHẤT LƯỢNG LÀM VIỆC TUẦN 4</t>
+  </si>
+  <si>
+    <t>13/10/2011 - 19/10/2011</t>
+  </si>
+  <si>
+    <t>Họ và Tên</t>
+  </si>
+  <si>
+    <t>Trịnh Anh Linh</t>
+  </si>
+  <si>
+    <t>Võ Anh Tuấn</t>
+  </si>
+  <si>
+    <t>Nguyễn Đinh Đình Bảo</t>
+  </si>
+  <si>
+    <t>Đánh giá chi tiết công việc</t>
+  </si>
+  <si>
+    <t>Đánh giá làm việc trong tuần cho từng thành viên</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Menu Manager'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Menu Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Menu Manager'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Menu Manager'</t>
+  </si>
+  <si>
+    <t>Khối lượng công việc</t>
+  </si>
+  <si>
+    <t>Trung bình</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Configuration'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Configuration'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Configuration'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Configuration'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Acticle Manager + Copy Acticle + Move Acticle + Global Configuration Pop-up Window'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Acticle Manager + Copy Acticle + Move Acticle + Global Configuration Pop-up Window'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Acticle Manager + Copy Acticle + Move Acticle + Global Configuration Pop-up Window'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Acticle Manager + Copy Acticle + Move Acticle + Global Configuration Pop-up Window'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Section Manager + Category Manager + Front Page Manager'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Section Manager + Category Manager + Front Page Manager'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Section Manager + Category Manager + Front Page Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Section Manager + Category Manager + Front Page Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Section Edit + Category Edit + Acticle Edit'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Section Edit + Category Edit + Acticle Edit'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Section Edit + Category Edit + Acticle Edit'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Section Edit + Category Edit + Acticle Edit'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'User Manager'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'User Manager'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'User Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'User Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'New User + Edit User'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'New User + Edit User'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'New User + Edit User'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'New User + Edit User'</t>
+  </si>
+  <si>
+    <t>Liệt kê tất cả control cần thiết cho màn hình 'Login + Language Manager'</t>
+  </si>
+  <si>
+    <t>Vẽ bố cục thiết kế sơ bộ màn hình 'Login + Language Manager'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Login + Language Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Login + Language Manager'</t>
+  </si>
+  <si>
+    <t>Demo login using PHP, MySQL</t>
+  </si>
+  <si>
+    <t>Study Book "How to build a full CMS" and give idea.</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Media Option'</t>
+  </si>
+  <si>
+    <t>Mapping DB cho màn hình 'Media Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Media Manager'</t>
+  </si>
+  <si>
+    <t>Liệt kê các sự kiện cần thiết cho màn hình 'Media Option'</t>
+  </si>
+  <si>
+    <t>Xây dựng bố cục project trong thư mục &lt;project_root&gt;/Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +310,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -203,11 +405,315 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -239,12 +745,118 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -323,6 +935,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +970,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,14 +1146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
@@ -551,7 +1165,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25">
+    <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
       <c r="D1" s="12" t="s">
         <v>19</v>
       </c>
@@ -561,7 +1175,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
@@ -581,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -599,7 +1213,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -623,7 +1237,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -645,7 +1259,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -667,7 +1281,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>4</v>
       </c>
@@ -689,7 +1303,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
@@ -711,7 +1325,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>6</v>
       </c>
@@ -733,7 +1347,7 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>7</v>
       </c>
@@ -755,7 +1369,7 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>8</v>
       </c>
@@ -777,7 +1391,7 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9</v>
       </c>
@@ -799,7 +1413,7 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>10</v>
       </c>
@@ -821,7 +1435,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
@@ -859,14 +1473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -876,7 +1490,7 @@
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -891,7 +1505,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -904,7 +1518,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="10" t="s">
         <v>17</v>
@@ -927,7 +1541,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="11"/>
       <c r="C4" s="6"/>
@@ -948,7 +1562,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
@@ -975,7 +1589,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
@@ -1000,7 +1614,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
@@ -1025,7 +1639,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
@@ -1050,7 +1664,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
@@ -1075,7 +1689,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
@@ -1100,7 +1714,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
@@ -1125,7 +1739,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
@@ -1150,7 +1764,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
@@ -1175,7 +1789,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
@@ -1200,7 +1814,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
@@ -1223,7 +1837,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1236,7 +1850,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1249,7 +1863,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1262,7 +1876,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1275,7 +1889,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1288,7 +1902,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1301,7 +1915,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1329,14 +1943,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -1346,7 +1960,7 @@
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1361,7 +1975,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1374,7 +1988,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="10" t="s">
         <v>17</v>
@@ -1397,7 +2011,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="11"/>
       <c r="C4" s="6"/>
@@ -1418,7 +2032,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
@@ -1445,7 +2059,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
@@ -1470,7 +2084,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
@@ -1495,7 +2109,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
@@ -1520,7 +2134,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
@@ -1545,7 +2159,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
@@ -1570,7 +2184,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
@@ -1595,7 +2209,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
@@ -1622,7 +2236,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
@@ -1647,7 +2261,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
@@ -1674,7 +2288,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
@@ -1699,7 +2313,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1712,7 +2326,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1725,7 +2339,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1738,7 +2352,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1751,7 +2365,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1764,7 +2378,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1777,7 +2391,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1802,4 +2416,1800 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M67"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="20" style="14" customWidth="1"/>
+    <col min="4" max="6" width="19.5703125" style="14" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="14" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="14" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <v>1</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="37">
+        <v>4</v>
+      </c>
+      <c r="D6" s="37">
+        <v>3</v>
+      </c>
+      <c r="E6" s="37">
+        <v>3</v>
+      </c>
+      <c r="F6" s="37">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="38">
+        <f>AVERAGE(C6:F6)</f>
+        <v>3.375</v>
+      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>2</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="39">
+        <v>4</v>
+      </c>
+      <c r="D7" s="39">
+        <v>3</v>
+      </c>
+      <c r="E7" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F7" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="40">
+        <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="29">
+        <v>3</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="39">
+        <v>4</v>
+      </c>
+      <c r="D8" s="39">
+        <v>3</v>
+      </c>
+      <c r="E8" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>4</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="39">
+        <v>5</v>
+      </c>
+      <c r="D9" s="39">
+        <v>3</v>
+      </c>
+      <c r="E9" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="40">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>5</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="39">
+        <v>4</v>
+      </c>
+      <c r="D10" s="39">
+        <v>3</v>
+      </c>
+      <c r="E10" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>6</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="39">
+        <v>4</v>
+      </c>
+      <c r="D11" s="39">
+        <v>3</v>
+      </c>
+      <c r="E11" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="29">
+        <v>7</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="39">
+        <v>4</v>
+      </c>
+      <c r="D12" s="39">
+        <v>3</v>
+      </c>
+      <c r="E12" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F12" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>8</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="39">
+        <v>4</v>
+      </c>
+      <c r="D13" s="39">
+        <v>3</v>
+      </c>
+      <c r="E13" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F13" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>9</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="39">
+        <v>4</v>
+      </c>
+      <c r="D14" s="39">
+        <v>3</v>
+      </c>
+      <c r="E14" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>10</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="39">
+        <v>4</v>
+      </c>
+      <c r="D15" s="39">
+        <v>3</v>
+      </c>
+      <c r="E15" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>11</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="39">
+        <v>4</v>
+      </c>
+      <c r="D16" s="39">
+        <v>3</v>
+      </c>
+      <c r="E16" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="40">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="30"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="28">
+        <v>1</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="55">
+        <v>40830</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37">
+        <v>4</v>
+      </c>
+      <c r="K22" s="37">
+        <v>3.5</v>
+      </c>
+      <c r="L22" s="37">
+        <v>3.5</v>
+      </c>
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>2</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39">
+        <v>4</v>
+      </c>
+      <c r="K23" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="22"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>3</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39">
+        <v>4</v>
+      </c>
+      <c r="K24" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M24" s="22"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="29">
+        <v>4</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39">
+        <v>4</v>
+      </c>
+      <c r="K25" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L25" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>5</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H26" s="21"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39">
+        <v>4</v>
+      </c>
+      <c r="K26" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L26" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M26" s="22"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>6</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39">
+        <v>4</v>
+      </c>
+      <c r="K27" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L27" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M27" s="22"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="29">
+        <v>7</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39">
+        <v>4</v>
+      </c>
+      <c r="K28" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L28" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M28" s="22"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39">
+        <v>4</v>
+      </c>
+      <c r="K29" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L29" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M29" s="22"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="29">
+        <v>9</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H30" s="21"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39">
+        <v>4</v>
+      </c>
+      <c r="K30" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L30" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M30" s="22"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="29">
+        <v>10</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H31" s="21"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39">
+        <v>4</v>
+      </c>
+      <c r="K31" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L31" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M31" s="22"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="29">
+        <v>11</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39">
+        <v>4</v>
+      </c>
+      <c r="K32" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L32" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M32" s="22"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="29">
+        <v>12</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H33" s="21"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39">
+        <v>4</v>
+      </c>
+      <c r="K33" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L33" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="29">
+        <v>13</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H34" s="21"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39">
+        <v>4</v>
+      </c>
+      <c r="K34" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L34" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="29">
+        <v>14</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H35" s="21"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39">
+        <v>4</v>
+      </c>
+      <c r="K35" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L35" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="29">
+        <v>15</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39">
+        <v>4</v>
+      </c>
+      <c r="K36" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L36" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M36" s="22"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="29">
+        <v>16</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H37" s="21"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39">
+        <v>4</v>
+      </c>
+      <c r="K37" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L37" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M37" s="22"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="29">
+        <v>17</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H38" s="21"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39">
+        <v>4</v>
+      </c>
+      <c r="K38" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L38" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M38" s="22"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="29">
+        <v>18</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H39" s="21"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39">
+        <v>4</v>
+      </c>
+      <c r="K39" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L39" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M39" s="22"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="29">
+        <v>19</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H40" s="21"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39">
+        <v>4</v>
+      </c>
+      <c r="K40" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L40" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M40" s="22"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="29">
+        <v>20</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H41" s="21"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39">
+        <v>4</v>
+      </c>
+      <c r="K41" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L41" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M41" s="22"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="29">
+        <v>21</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H42" s="21"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39">
+        <v>4</v>
+      </c>
+      <c r="K42" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L42" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M42" s="22"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="29">
+        <v>22</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H43" s="21"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39">
+        <v>4</v>
+      </c>
+      <c r="K43" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L43" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M43" s="22"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="29">
+        <v>23</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H44" s="21"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39">
+        <v>4</v>
+      </c>
+      <c r="K44" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L44" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M44" s="22"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="29">
+        <v>24</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H45" s="21"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39">
+        <v>4</v>
+      </c>
+      <c r="K45" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L45" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M45" s="22"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="29">
+        <v>25</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H46" s="21"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39">
+        <v>4</v>
+      </c>
+      <c r="K46" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L46" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M46" s="22"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="29">
+        <v>26</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H47" s="21"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39">
+        <v>4</v>
+      </c>
+      <c r="K47" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L47" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M47" s="22"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="29">
+        <v>27</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H48" s="21"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39">
+        <v>4</v>
+      </c>
+      <c r="K48" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L48" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M48" s="22"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="29">
+        <v>28</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H49" s="21"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39">
+        <v>4</v>
+      </c>
+      <c r="K49" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L49" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M49" s="22"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="29">
+        <v>29</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H50" s="21"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39">
+        <v>4</v>
+      </c>
+      <c r="K50" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L50" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M50" s="22"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="29">
+        <v>30</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H51" s="21"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="39">
+        <v>4</v>
+      </c>
+      <c r="K51" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L51" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M51" s="22"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="29">
+        <v>31</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H52" s="21"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39">
+        <v>4</v>
+      </c>
+      <c r="K52" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L52" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M52" s="22"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="29">
+        <v>32</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H53" s="21"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="39">
+        <v>4</v>
+      </c>
+      <c r="K53" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L53" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M53" s="22"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="29">
+        <v>33</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H54" s="21"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39">
+        <v>4</v>
+      </c>
+      <c r="K54" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L54" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M54" s="22"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="29">
+        <v>34</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H55" s="21"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39">
+        <v>4</v>
+      </c>
+      <c r="K55" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L55" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M55" s="22"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="29">
+        <v>35</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H56" s="21"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39">
+        <v>4</v>
+      </c>
+      <c r="K56" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L56" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M56" s="22"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="29">
+        <v>36</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H57" s="21"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39">
+        <v>4</v>
+      </c>
+      <c r="K57" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L57" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M57" s="22"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="29">
+        <v>37</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="56">
+        <v>40830</v>
+      </c>
+      <c r="H58" s="21"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39">
+        <v>4</v>
+      </c>
+      <c r="K58" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L58" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M58" s="22"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="29">
+        <v>38</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="56">
+        <v>40833</v>
+      </c>
+      <c r="H59" s="21"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39">
+        <v>4</v>
+      </c>
+      <c r="K59" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L59" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M59" s="22"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="29">
+        <v>39</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="56">
+        <v>40834</v>
+      </c>
+      <c r="H60" s="21"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39">
+        <v>4</v>
+      </c>
+      <c r="K60" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L60" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M60" s="22"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="29">
+        <v>40</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H61" s="21"/>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39">
+        <v>4</v>
+      </c>
+      <c r="K61" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L61" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M61" s="22"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="29">
+        <v>41</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="56">
+        <v>40835</v>
+      </c>
+      <c r="H62" s="21"/>
+      <c r="I62" s="39"/>
+      <c r="J62" s="39">
+        <v>5</v>
+      </c>
+      <c r="K62" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="L62" s="39">
+        <v>3.5</v>
+      </c>
+      <c r="M62" s="22"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="29"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="22"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="29"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="39"/>
+      <c r="L64" s="39"/>
+      <c r="M64" s="22"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="29"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="39"/>
+      <c r="J65" s="39"/>
+      <c r="K65" s="39"/>
+      <c r="L65" s="39"/>
+      <c r="M65" s="22"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="29"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="56"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="39"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="39"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="22"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="30"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="57"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="41"/>
+      <c r="K67" s="41"/>
+      <c r="L67" s="41"/>
+      <c r="M67" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B20:G21">
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+  </autoFilter>
+  <mergeCells count="9">
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="C20:F21"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
câp nhật đánh giá thành viên ngày 19.10.2011
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="3"/>
@@ -16,12 +16,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuần 4'!$B$20:$G$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Tuần 4'!$A$1:$M$67</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
   <si>
     <t>Task</t>
   </si>
@@ -274,20 +274,23 @@
   </si>
   <si>
     <t>Xây dựng bố cục project trong thư mục &lt;project_root&gt;/Source</t>
+  </si>
+  <si>
+    <t>chưa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -713,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -724,34 +727,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -782,24 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,15 +795,61 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,7 +939,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -970,7 +973,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1146,59 +1148,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.125" style="1"/>
+    <col min="3" max="3" width="12.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="2:9" ht="20.25">
+      <c r="D1" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:9">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+    <row r="4" spans="2:9">
+      <c r="B4" s="49"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1211,13 +1213,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="45" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1237,11 +1239,11 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1259,11 +1261,11 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1281,11 +1283,11 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1303,11 +1305,11 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1325,11 +1327,11 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1347,11 +1349,11 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1369,11 +1371,11 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1391,11 +1393,11 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1413,11 +1415,11 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1435,11 +1437,11 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1473,31 +1475,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.875" customWidth="1"/>
+    <col min="8" max="8" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="20.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1505,7 +1507,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1518,34 +1520,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1"/>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1558,16 +1560,16 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1589,12 +1591,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1614,12 +1616,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1639,12 +1641,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1664,12 +1666,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1689,12 +1691,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1714,12 +1716,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1739,12 +1741,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1764,12 +1766,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1789,12 +1791,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1814,12 +1816,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1837,7 +1839,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1850,7 +1852,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1863,7 +1865,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1876,7 +1878,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1889,7 +1891,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1902,7 +1904,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1915,7 +1917,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1943,31 +1945,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.875" customWidth="1"/>
+    <col min="8" max="8" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="20.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1975,7 +1977,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1988,34 +1990,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1"/>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2028,16 +2030,16 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="45" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2059,12 +2061,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2084,12 +2086,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2109,12 +2111,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2134,12 +2136,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2159,12 +2161,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2184,12 +2186,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2209,12 +2211,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2236,12 +2238,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2261,12 +2263,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2288,12 +2290,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2313,7 +2315,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2326,7 +2328,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2339,7 +2341,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2352,7 +2354,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2365,7 +2367,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2378,7 +2380,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2391,7 +2393,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2419,1778 +2421,1840 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="20" style="14" customWidth="1"/>
-    <col min="4" max="6" width="19.5703125" style="14" customWidth="1"/>
-    <col min="7" max="12" width="12.140625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" style="14" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="4.375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20" style="6" customWidth="1"/>
+    <col min="4" max="6" width="19.625" style="6" customWidth="1"/>
+    <col min="7" max="12" width="12.125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="28.125" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+    <row r="2" spans="1:13" ht="15.75">
+      <c r="A2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25">
+      <c r="A3" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-    </row>
-    <row r="5" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" s="17" customFormat="1">
+      <c r="A5" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+    <row r="6" spans="1:13">
+      <c r="A6" s="19">
         <v>1</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="37">
-        <v>4</v>
-      </c>
-      <c r="D6" s="37">
+      <c r="C6" s="22">
+        <v>4</v>
+      </c>
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="22">
         <v>3</v>
       </c>
-      <c r="F6" s="37">
-        <v>3.5</v>
-      </c>
-      <c r="G6" s="38">
+      <c r="F6" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="23">
         <f>AVERAGE(C6:F6)</f>
         <v>3.375</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="39">
-        <v>4</v>
-      </c>
-      <c r="D7" s="39">
+      <c r="C7" s="24">
+        <v>4</v>
+      </c>
+      <c r="D7" s="24">
         <v>3</v>
       </c>
-      <c r="E7" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F7" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G7" s="40">
+      <c r="E7" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F7" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="25">
         <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
         <v>3.5</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="20">
         <v>3</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="39">
-        <v>4</v>
-      </c>
-      <c r="D8" s="39">
+      <c r="C8" s="24">
+        <v>4</v>
+      </c>
+      <c r="D8" s="24">
         <v>3</v>
       </c>
-      <c r="E8" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F8" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G8" s="40">
+      <c r="E8" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
-        <v>4</v>
-      </c>
-      <c r="B9" s="44" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="24">
         <v>5</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="24">
         <v>3</v>
       </c>
-      <c r="E9" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F9" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G9" s="40">
+      <c r="E9" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="39">
-        <v>4</v>
-      </c>
-      <c r="D10" s="39">
+      <c r="C10" s="24">
+        <v>4</v>
+      </c>
+      <c r="D10" s="24">
         <v>3</v>
       </c>
-      <c r="E10" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F10" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G10" s="40">
+      <c r="E10" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="29">
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="39">
-        <v>4</v>
-      </c>
-      <c r="D11" s="39">
+      <c r="C11" s="24">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24">
         <v>3</v>
       </c>
-      <c r="E11" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G11" s="40">
+      <c r="E11" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="20">
         <v>7</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="39">
-        <v>4</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="C12" s="24">
+        <v>4</v>
+      </c>
+      <c r="D12" s="24">
         <v>3</v>
       </c>
-      <c r="E12" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G12" s="40">
+      <c r="E12" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F12" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="20">
         <v>8</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="39">
-        <v>4</v>
-      </c>
-      <c r="D13" s="39">
+      <c r="C13" s="24">
+        <v>4</v>
+      </c>
+      <c r="D13" s="24">
         <v>3</v>
       </c>
-      <c r="E13" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F13" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G13" s="40">
+      <c r="E13" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F13" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="29">
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="20">
         <v>9</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="39">
-        <v>4</v>
-      </c>
-      <c r="D14" s="39">
+      <c r="C14" s="24">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24">
         <v>3</v>
       </c>
-      <c r="E14" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G14" s="40">
+      <c r="E14" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="29">
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="20">
         <v>10</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="39">
-        <v>4</v>
-      </c>
-      <c r="D15" s="39">
+      <c r="C15" s="24">
+        <v>4</v>
+      </c>
+      <c r="D15" s="24">
         <v>3</v>
       </c>
-      <c r="E15" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F15" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G15" s="40">
+      <c r="E15" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="29">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="20">
         <v>11</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="39">
-        <v>4</v>
-      </c>
-      <c r="D16" s="39">
+      <c r="C16" s="24">
+        <v>4</v>
+      </c>
+      <c r="D16" s="24">
         <v>3</v>
       </c>
-      <c r="E16" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F16" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="G16" s="40">
+      <c r="E16" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="25">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="21"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="15" t="s">
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15" t="s">
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="17" t="s">
+    <row r="21" spans="1:13" s="9" customFormat="1">
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="17" t="s">
+      <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="28">
+      <c r="M21" s="51"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="19">
         <v>1</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="55">
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="40">
         <v>40830</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37">
-        <v>4</v>
-      </c>
-      <c r="K22" s="37">
-        <v>3.5</v>
-      </c>
-      <c r="L22" s="37">
-        <v>3.5</v>
-      </c>
-      <c r="M22" s="20"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="29">
+      <c r="H22" s="10"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22">
+        <v>4</v>
+      </c>
+      <c r="K22" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="L22" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="20">
         <v>2</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="56">
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="41">
         <v>40833</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39">
-        <v>4</v>
-      </c>
-      <c r="K23" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L23" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M23" s="22"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
+      <c r="H23" s="12"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24">
+        <v>4</v>
+      </c>
+      <c r="K23" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="20">
         <v>3</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="56">
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="41">
         <v>40834</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39">
-        <v>4</v>
-      </c>
-      <c r="K24" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L24" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M24" s="22"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="29">
-        <v>4</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="H24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24">
+        <v>4</v>
+      </c>
+      <c r="K24" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M24" s="13"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="20">
+        <v>4</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="56">
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="41">
         <v>40835</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39">
-        <v>4</v>
-      </c>
-      <c r="K25" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L25" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M25" s="22"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="29">
+      <c r="H25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24">
+        <v>4</v>
+      </c>
+      <c r="K25" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L25" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="20">
         <v>5</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="56">
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="41">
         <v>40830</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39">
-        <v>4</v>
-      </c>
-      <c r="K26" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L26" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
+      <c r="H26" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24">
+        <v>4</v>
+      </c>
+      <c r="K26" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L26" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M26" s="13"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="20">
         <v>6</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="56">
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="41">
         <v>40833</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39">
-        <v>4</v>
-      </c>
-      <c r="K27" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L27" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M27" s="22"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="29">
+      <c r="H27" s="60">
+        <v>40831</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24">
+        <v>4</v>
+      </c>
+      <c r="K27" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L27" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="20">
         <v>7</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="56">
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="41">
         <v>40834</v>
       </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39">
-        <v>4</v>
-      </c>
-      <c r="K28" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L28" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M28" s="22"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="29">
+      <c r="H28" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24">
+        <v>4</v>
+      </c>
+      <c r="K28" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L28" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M28" s="13"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="20">
         <v>8</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="56">
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="41">
         <v>40835</v>
       </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39">
-        <v>4</v>
-      </c>
-      <c r="K29" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L29" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M29" s="22"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="29">
+      <c r="H29" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24">
+        <v>4</v>
+      </c>
+      <c r="K29" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L29" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M29" s="13"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="20">
         <v>9</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="56">
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="41">
         <v>40830</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39">
-        <v>4</v>
-      </c>
-      <c r="K30" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L30" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M30" s="22"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="29">
+      <c r="H30" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24">
+        <v>4</v>
+      </c>
+      <c r="K30" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L30" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M30" s="13"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="20">
         <v>10</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="56">
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="41">
         <v>40833</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39">
-        <v>4</v>
-      </c>
-      <c r="K31" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L31" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M31" s="22"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="29">
+      <c r="H31" s="60">
+        <v>40833</v>
+      </c>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24">
+        <v>4</v>
+      </c>
+      <c r="K31" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L31" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="20">
         <v>11</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="56">
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="41">
         <v>40834</v>
       </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39">
-        <v>4</v>
-      </c>
-      <c r="K32" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L32" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M32" s="22"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="29">
+      <c r="H32" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24">
+        <v>4</v>
+      </c>
+      <c r="K32" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L32" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="20">
         <v>12</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="56">
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="41">
         <v>40835</v>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39">
-        <v>4</v>
-      </c>
-      <c r="K33" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L33" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M33" s="22"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="29">
+      <c r="H33" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24">
+        <v>4</v>
+      </c>
+      <c r="K33" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L33" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="20">
         <v>13</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="56">
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="41">
         <v>40830</v>
       </c>
-      <c r="H34" s="21"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39">
-        <v>4</v>
-      </c>
-      <c r="K34" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L34" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M34" s="22"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="29">
+      <c r="H34" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24">
+        <v>4</v>
+      </c>
+      <c r="K34" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L34" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="20">
         <v>14</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="56">
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="41">
         <v>40833</v>
       </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39">
-        <v>4</v>
-      </c>
-      <c r="K35" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L35" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M35" s="22"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="29">
+      <c r="H35" s="60">
+        <v>40833</v>
+      </c>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24">
+        <v>4</v>
+      </c>
+      <c r="K35" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L35" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="20">
         <v>15</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="56">
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="41">
         <v>40834</v>
       </c>
-      <c r="H36" s="21"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39">
-        <v>4</v>
-      </c>
-      <c r="K36" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L36" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M36" s="22"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="29">
+      <c r="H36" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24">
+        <v>4</v>
+      </c>
+      <c r="K36" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L36" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="20">
         <v>16</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="56">
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="41">
         <v>40835</v>
       </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39">
-        <v>4</v>
-      </c>
-      <c r="K37" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L37" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M37" s="22"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="29">
+      <c r="H37" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24">
+        <v>4</v>
+      </c>
+      <c r="K37" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L37" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="20">
         <v>17</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="56">
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="41">
         <v>40830</v>
       </c>
-      <c r="H38" s="21"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39">
-        <v>4</v>
-      </c>
-      <c r="K38" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L38" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M38" s="22"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="29">
+      <c r="H38" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24">
+        <v>4</v>
+      </c>
+      <c r="K38" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L38" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="20">
         <v>18</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="56">
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="41">
         <v>40833</v>
       </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39">
-        <v>4</v>
-      </c>
-      <c r="K39" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L39" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M39" s="22"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="29">
+      <c r="H39" s="60">
+        <v>40832</v>
+      </c>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24">
+        <v>4</v>
+      </c>
+      <c r="K39" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L39" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="20">
         <v>19</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="56">
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="41">
         <v>40834</v>
       </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39">
-        <v>4</v>
-      </c>
-      <c r="K40" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L40" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M40" s="22"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="29">
+      <c r="H40" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24">
+        <v>4</v>
+      </c>
+      <c r="K40" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L40" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="20">
         <v>20</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="56">
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="41">
         <v>40835</v>
       </c>
-      <c r="H41" s="21"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39">
-        <v>4</v>
-      </c>
-      <c r="K41" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L41" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M41" s="22"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="29">
+      <c r="H41" s="60">
+        <v>40834</v>
+      </c>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24">
+        <v>4</v>
+      </c>
+      <c r="K41" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L41" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="20">
         <v>21</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="56">
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="41">
         <v>40830</v>
       </c>
-      <c r="H42" s="21"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39">
-        <v>4</v>
-      </c>
-      <c r="K42" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L42" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M42" s="22"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="29">
+      <c r="H42" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24">
+        <v>4</v>
+      </c>
+      <c r="K42" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L42" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="20">
         <v>22</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="56">
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="41">
         <v>40833</v>
       </c>
-      <c r="H43" s="21"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39">
-        <v>4</v>
-      </c>
-      <c r="K43" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L43" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M43" s="22"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="29">
+      <c r="H43" s="60">
+        <v>40832</v>
+      </c>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24">
+        <v>4</v>
+      </c>
+      <c r="K43" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L43" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="20">
         <v>23</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="56">
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="41">
         <v>40834</v>
       </c>
-      <c r="H44" s="21"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39">
-        <v>4</v>
-      </c>
-      <c r="K44" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L44" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M44" s="22"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="29">
+      <c r="H44" s="60">
+        <v>40832</v>
+      </c>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24">
+        <v>4</v>
+      </c>
+      <c r="K44" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L44" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="20">
         <v>24</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="56">
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="41">
         <v>40835</v>
       </c>
-      <c r="H45" s="21"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39">
-        <v>4</v>
-      </c>
-      <c r="K45" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L45" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M45" s="22"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="29">
+      <c r="H45" s="60">
+        <v>40832</v>
+      </c>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24">
+        <v>4</v>
+      </c>
+      <c r="K45" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L45" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="20">
         <v>25</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="49" t="s">
+      <c r="C46" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="56">
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="41">
         <v>40830</v>
       </c>
-      <c r="H46" s="21"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39">
-        <v>4</v>
-      </c>
-      <c r="K46" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L46" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M46" s="22"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="29">
+      <c r="H46" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24">
+        <v>4</v>
+      </c>
+      <c r="K46" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L46" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="20">
         <v>26</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="56">
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="41">
         <v>40833</v>
       </c>
-      <c r="H47" s="21"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39">
-        <v>4</v>
-      </c>
-      <c r="K47" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L47" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M47" s="22"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="29">
+      <c r="H47" s="60">
+        <v>40832</v>
+      </c>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24">
+        <v>4</v>
+      </c>
+      <c r="K47" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L47" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M47" s="13"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="20">
         <v>27</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="49" t="s">
+      <c r="C48" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="56">
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="41">
         <v>40834</v>
       </c>
-      <c r="H48" s="21"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39">
-        <v>4</v>
-      </c>
-      <c r="K48" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L48" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M48" s="22"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="29">
+      <c r="H48" s="60">
+        <v>40833</v>
+      </c>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24">
+        <v>4</v>
+      </c>
+      <c r="K48" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L48" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M48" s="13"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="20">
         <v>28</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="56">
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="41">
         <v>40835</v>
       </c>
-      <c r="H49" s="21"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39">
-        <v>4</v>
-      </c>
-      <c r="K49" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L49" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M49" s="22"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="29">
+      <c r="H49" s="60">
+        <v>40833</v>
+      </c>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24">
+        <v>4</v>
+      </c>
+      <c r="K49" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L49" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M49" s="13"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="20">
         <v>29</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="49" t="s">
+      <c r="C50" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="56">
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="41">
         <v>40830</v>
       </c>
-      <c r="H50" s="21"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39">
-        <v>4</v>
-      </c>
-      <c r="K50" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L50" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M50" s="22"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="29">
+      <c r="H50" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24">
+        <v>4</v>
+      </c>
+      <c r="K50" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L50" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M50" s="13"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="20">
         <v>30</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="56">
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="41">
         <v>40833</v>
       </c>
-      <c r="H51" s="21"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39">
-        <v>4</v>
-      </c>
-      <c r="K51" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L51" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M51" s="22"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="29">
+      <c r="H51" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24">
+        <v>4</v>
+      </c>
+      <c r="K51" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L51" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M51" s="13"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="20">
         <v>31</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="56">
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="41">
         <v>40834</v>
       </c>
-      <c r="H52" s="21"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39">
-        <v>4</v>
-      </c>
-      <c r="K52" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L52" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M52" s="22"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="29">
+      <c r="H52" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24">
+        <v>4</v>
+      </c>
+      <c r="K52" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L52" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M52" s="13"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="20">
         <v>32</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="56">
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="41">
         <v>40835</v>
       </c>
-      <c r="H53" s="21"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39">
-        <v>4</v>
-      </c>
-      <c r="K53" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L53" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M53" s="22"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="29">
+      <c r="H53" s="60">
+        <v>40830</v>
+      </c>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24">
+        <v>4</v>
+      </c>
+      <c r="K53" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L53" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M53" s="13"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="20">
         <v>33</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="56">
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="41">
         <v>40830</v>
       </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39">
-        <v>4</v>
-      </c>
-      <c r="K54" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L54" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M54" s="22"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="29">
+      <c r="H54" s="12"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24">
+        <v>4</v>
+      </c>
+      <c r="K54" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L54" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M54" s="13"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="20">
         <v>34</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="56">
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="41">
         <v>40833</v>
       </c>
-      <c r="H55" s="21"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39">
-        <v>4</v>
-      </c>
-      <c r="K55" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L55" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M55" s="22"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="29">
+      <c r="H55" s="12"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24">
+        <v>4</v>
+      </c>
+      <c r="K55" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L55" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M55" s="13"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="20">
         <v>35</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="56">
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="41">
         <v>40834</v>
       </c>
-      <c r="H56" s="21"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39">
-        <v>4</v>
-      </c>
-      <c r="K56" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L56" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M56" s="22"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="29">
+      <c r="H56" s="12"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24">
+        <v>4</v>
+      </c>
+      <c r="K56" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L56" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M56" s="13"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="20">
         <v>36</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="51"/>
-      <c r="G57" s="56">
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="41">
         <v>40835</v>
       </c>
-      <c r="H57" s="21"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39">
-        <v>4</v>
-      </c>
-      <c r="K57" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L57" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M57" s="22"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="29">
+      <c r="H57" s="12"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24">
+        <v>4</v>
+      </c>
+      <c r="K57" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L57" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M57" s="13"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="20">
         <v>37</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="51"/>
-      <c r="G58" s="56">
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="41">
         <v>40830</v>
       </c>
-      <c r="H58" s="21"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39">
-        <v>4</v>
-      </c>
-      <c r="K58" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L58" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M58" s="22"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="29">
+      <c r="H58" s="12"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24">
+        <v>4</v>
+      </c>
+      <c r="K58" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L58" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M58" s="13"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="20">
         <v>38</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="56">
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="41">
         <v>40833</v>
       </c>
-      <c r="H59" s="21"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39">
-        <v>4</v>
-      </c>
-      <c r="K59" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L59" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M59" s="22"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="29">
+      <c r="H59" s="12"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="24">
+        <v>4</v>
+      </c>
+      <c r="K59" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L59" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M59" s="13"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="20">
         <v>39</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="56">
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="41">
         <v>40834</v>
       </c>
-      <c r="H60" s="21"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39">
-        <v>4</v>
-      </c>
-      <c r="K60" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L60" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M60" s="22"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="29">
+      <c r="H60" s="12"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="24">
+        <v>4</v>
+      </c>
+      <c r="K60" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L60" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M60" s="13"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="20">
         <v>40</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="49" t="s">
+      <c r="C61" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="56">
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="41">
         <v>40835</v>
       </c>
-      <c r="H61" s="21"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39">
-        <v>4</v>
-      </c>
-      <c r="K61" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L61" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M61" s="22"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="29">
+      <c r="H61" s="12"/>
+      <c r="I61" s="24"/>
+      <c r="J61" s="24">
+        <v>4</v>
+      </c>
+      <c r="K61" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L61" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M61" s="13"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="20">
         <v>41</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="49" t="s">
+      <c r="C62" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="51"/>
-      <c r="G62" s="56">
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="41">
         <v>40835</v>
       </c>
-      <c r="H62" s="21"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39">
+      <c r="H62" s="60">
+        <v>40835</v>
+      </c>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24">
         <v>5</v>
       </c>
-      <c r="K62" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="L62" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="M62" s="22"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="29"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="51"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
-      <c r="M63" s="22"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="51"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="22"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="29"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="22"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="29"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="51"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="22"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="30"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="57"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="41"/>
-      <c r="L67" s="41"/>
-      <c r="M67" s="24"/>
+      <c r="K62" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="L62" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="M62" s="13"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="20"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="13"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="20"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="24"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="24"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="13"/>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="20"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="24"/>
+      <c r="J65" s="24"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="24"/>
+      <c r="M65" s="13"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="20"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="24"/>
+      <c r="L66" s="24"/>
+      <c r="M66" s="13"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="21"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="B20:G21">

</xml_diff>

<commit_message>
Evalue project member's work in week 4.
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="3"/>
@@ -13,15 +13,15 @@
     <sheet name="Tuần 4" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuần 4'!$B$20:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuần 4'!$B$20:$G$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Tuần 4'!$A$1:$M$67</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>Task</t>
   </si>
@@ -274,23 +274,20 @@
   </si>
   <si>
     <t>Xây dựng bố cục project trong thư mục &lt;project_root&gt;/Source</t>
-  </si>
-  <si>
-    <t>chưa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -716,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -762,19 +759,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -849,7 +837,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,6 +935,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -973,6 +970,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1148,59 +1146,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="12.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25">
-      <c r="D1" s="50" t="s">
+    <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="48" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1213,13 +1211,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1239,11 +1237,11 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1261,11 +1259,11 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1283,11 +1281,11 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1305,11 +1303,11 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1327,11 +1325,11 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1349,11 +1347,11 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1371,11 +1369,11 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1393,11 +1391,11 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1415,11 +1413,11 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1437,11 +1435,11 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1475,31 +1473,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1507,7 +1505,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1520,34 +1518,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1560,16 +1558,16 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1591,12 +1589,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1616,12 +1614,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1641,12 +1639,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1666,12 +1664,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1691,12 +1689,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1716,12 +1714,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1741,12 +1739,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1766,12 +1764,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1791,12 +1789,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1816,12 +1814,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1839,7 +1837,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1852,7 +1850,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1865,7 +1863,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1878,7 +1876,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1891,7 +1889,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1904,7 +1902,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1917,7 +1915,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1945,31 +1943,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1977,7 +1975,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1990,34 +1988,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2030,16 +2028,16 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2061,12 +2059,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2086,12 +2084,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2111,12 +2109,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2136,12 +2134,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2161,12 +2159,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2186,12 +2184,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2211,12 +2209,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2238,12 +2236,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2263,12 +2261,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2290,12 +2288,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2315,7 +2313,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2328,7 +2326,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2341,7 +2339,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2354,7 +2352,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2367,7 +2365,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2380,7 +2378,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2393,7 +2391,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2421,59 +2419,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="20" style="6" customWidth="1"/>
-    <col min="4" max="6" width="19.625" style="6" customWidth="1"/>
-    <col min="7" max="12" width="12.125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="28.125" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="6"/>
+    <col min="4" max="6" width="19.5703125" style="6" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.25">
-      <c r="A3" s="53" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
@@ -2490,41 +2488,41 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="22">
         <v>4</v>
       </c>
       <c r="D6" s="22">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E6" s="22">
         <v>3</v>
@@ -2532,9 +2530,9 @@
       <c r="F6" s="22">
         <v>3.5</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="57">
         <f>AVERAGE(C6:F6)</f>
-        <v>3.375</v>
+        <v>3.5</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -2543,28 +2541,28 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="24">
-        <v>4</v>
-      </c>
-      <c r="D7" s="24">
-        <v>3</v>
-      </c>
-      <c r="E7" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F7" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G7" s="25">
+      <c r="C7" s="23">
+        <v>4</v>
+      </c>
+      <c r="D7" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="23">
+        <v>3.25</v>
+      </c>
+      <c r="F7" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="58">
         <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
-        <v>3.5</v>
+        <v>3.5625</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -2573,28 +2571,28 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="24">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24">
-        <v>3</v>
-      </c>
-      <c r="E8" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F8" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G8" s="25">
+      <c r="C8" s="23">
+        <v>4</v>
+      </c>
+      <c r="D8" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="23">
+        <v>3.25</v>
+      </c>
+      <c r="F8" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.5625</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -2603,28 +2601,28 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>4</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>5</v>
       </c>
-      <c r="D9" s="24">
-        <v>3</v>
-      </c>
-      <c r="E9" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F9" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G9" s="25">
+      <c r="D9" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="58">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.875</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -2633,28 +2631,28 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="24">
-        <v>4</v>
-      </c>
-      <c r="D10" s="24">
-        <v>3</v>
-      </c>
-      <c r="E10" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F10" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G10" s="25">
+      <c r="C10" s="23">
+        <v>4</v>
+      </c>
+      <c r="D10" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E10" s="23">
+        <v>4</v>
+      </c>
+      <c r="F10" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
@@ -2663,28 +2661,28 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="24">
-        <v>4</v>
-      </c>
-      <c r="D11" s="24">
-        <v>3</v>
-      </c>
-      <c r="E11" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G11" s="25">
+      <c r="C11" s="23">
+        <v>4</v>
+      </c>
+      <c r="D11" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="23">
+        <v>3.75</v>
+      </c>
+      <c r="F11" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.6875</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -2693,28 +2691,28 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>7</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="24">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24">
-        <v>3</v>
-      </c>
-      <c r="E12" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G12" s="25">
+      <c r="C12" s="23">
+        <v>4</v>
+      </c>
+      <c r="D12" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E12" s="23">
+        <v>3.65</v>
+      </c>
+      <c r="F12" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.6625000000000001</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -2723,28 +2721,28 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>8</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="24">
-        <v>4</v>
-      </c>
-      <c r="D13" s="24">
-        <v>3</v>
-      </c>
-      <c r="E13" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F13" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G13" s="25">
+      <c r="C13" s="23">
+        <v>4</v>
+      </c>
+      <c r="D13" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2.75</v>
+      </c>
+      <c r="F13" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.4375</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -2753,28 +2751,28 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>9</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="24">
-        <v>4</v>
-      </c>
-      <c r="D14" s="24">
-        <v>3</v>
-      </c>
-      <c r="E14" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G14" s="25">
+      <c r="C14" s="23">
+        <v>4</v>
+      </c>
+      <c r="D14" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.625</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -2783,28 +2781,28 @@
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>10</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="24">
-        <v>4</v>
-      </c>
-      <c r="D15" s="24">
-        <v>3</v>
-      </c>
-      <c r="E15" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F15" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G15" s="25">
+      <c r="C15" s="23">
+        <v>4</v>
+      </c>
+      <c r="D15" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="23">
+        <v>3.85</v>
+      </c>
+      <c r="F15" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.7124999999999999</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -2813,28 +2811,28 @@
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>11</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="24">
-        <v>4</v>
-      </c>
-      <c r="D16" s="24">
-        <v>3</v>
-      </c>
-      <c r="E16" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="F16" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="G16" s="25">
+      <c r="C16" s="23">
+        <v>4</v>
+      </c>
+      <c r="D16" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="58">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.625</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -2843,14 +2841,14 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
@@ -2858,7 +2856,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2873,49 +2871,49 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="51" t="s">
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="51" t="s">
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="51" t="s">
+      <c r="I20" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51" t="s">
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="9" customFormat="1">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+    <row r="21" spans="1:13" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
@@ -2928,26 +2926,30 @@
       <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="51"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="M21" s="48"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="40">
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="37">
         <v>40830</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="22"/>
+      <c r="H22" s="37">
+        <v>40830</v>
+      </c>
+      <c r="I22" s="22">
+        <v>3</v>
+      </c>
       <c r="J22" s="22">
         <v>4</v>
       </c>
@@ -2959,966 +2961,1030 @@
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>2</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="41">
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="38">
         <v>40833</v>
       </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24">
-        <v>4</v>
-      </c>
-      <c r="K23" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L23" s="24">
+      <c r="H23" s="38">
+        <v>40832</v>
+      </c>
+      <c r="I23" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="23">
+        <v>4</v>
+      </c>
+      <c r="K23" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="23">
         <v>3.5</v>
       </c>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>3</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="41">
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="38">
         <v>40834</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24">
-        <v>4</v>
-      </c>
-      <c r="K24" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L24" s="24">
+      <c r="H24" s="38">
+        <v>40835</v>
+      </c>
+      <c r="I24" s="23">
+        <v>2</v>
+      </c>
+      <c r="J24" s="23">
+        <v>4</v>
+      </c>
+      <c r="K24" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="23">
         <v>3.5</v>
       </c>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>4</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="41">
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="38">
         <v>40835</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24">
-        <v>4</v>
-      </c>
-      <c r="K25" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L25" s="24">
+      <c r="H25" s="38">
+        <v>40835</v>
+      </c>
+      <c r="I25" s="23">
+        <v>2</v>
+      </c>
+      <c r="J25" s="23">
+        <v>4</v>
+      </c>
+      <c r="K25" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L25" s="23">
         <v>3.5</v>
       </c>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>5</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="41">
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="38">
         <v>40830</v>
       </c>
-      <c r="H26" s="60">
+      <c r="H26" s="38">
         <v>40830</v>
       </c>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24">
-        <v>4</v>
-      </c>
-      <c r="K26" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L26" s="24">
+      <c r="I26" s="23">
+        <v>3</v>
+      </c>
+      <c r="J26" s="23">
+        <v>4</v>
+      </c>
+      <c r="K26" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L26" s="23">
         <v>3.5</v>
       </c>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>6</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="41">
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="38">
         <v>40833</v>
       </c>
-      <c r="H27" s="60">
+      <c r="H27" s="38">
         <v>40831</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24">
-        <v>4</v>
-      </c>
-      <c r="K27" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L27" s="24">
+      <c r="I27" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="J27" s="23">
+        <v>4</v>
+      </c>
+      <c r="K27" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L27" s="23">
         <v>3.5</v>
       </c>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>7</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="41">
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="38">
         <v>40834</v>
       </c>
-      <c r="H28" s="60">
+      <c r="H28" s="38">
         <v>40834</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24">
-        <v>4</v>
-      </c>
-      <c r="K28" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L28" s="24">
+      <c r="I28" s="23">
+        <v>3</v>
+      </c>
+      <c r="J28" s="23">
+        <v>4</v>
+      </c>
+      <c r="K28" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L28" s="23">
         <v>3.5</v>
       </c>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>8</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="41">
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="38">
         <v>40835</v>
       </c>
-      <c r="H29" s="60">
+      <c r="H29" s="38">
         <v>40834</v>
       </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24">
-        <v>4</v>
-      </c>
-      <c r="K29" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L29" s="24">
+      <c r="I29" s="23">
+        <v>4</v>
+      </c>
+      <c r="J29" s="23">
+        <v>4</v>
+      </c>
+      <c r="K29" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L29" s="23">
         <v>3.5</v>
       </c>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>9</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="41">
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="38">
         <v>40830</v>
       </c>
-      <c r="H30" s="60">
+      <c r="H30" s="38">
         <v>40830</v>
       </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24">
-        <v>4</v>
-      </c>
-      <c r="K30" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L30" s="24">
+      <c r="I30" s="23">
+        <v>3</v>
+      </c>
+      <c r="J30" s="23">
+        <v>4</v>
+      </c>
+      <c r="K30" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L30" s="23">
         <v>3.5</v>
       </c>
       <c r="M30" s="13"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>10</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="41">
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="38">
         <v>40833</v>
       </c>
-      <c r="H31" s="60">
+      <c r="H31" s="38">
         <v>40833</v>
       </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24">
-        <v>4</v>
-      </c>
-      <c r="K31" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L31" s="24">
+      <c r="I31" s="23">
+        <v>3</v>
+      </c>
+      <c r="J31" s="23">
+        <v>4</v>
+      </c>
+      <c r="K31" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L31" s="23">
         <v>3.5</v>
       </c>
       <c r="M31" s="13"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>11</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="41">
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="38">
         <v>40834</v>
       </c>
-      <c r="H32" s="60">
+      <c r="H32" s="38">
         <v>40834</v>
       </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24">
-        <v>4</v>
-      </c>
-      <c r="K32" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L32" s="24">
+      <c r="I32" s="23">
+        <v>3</v>
+      </c>
+      <c r="J32" s="23">
+        <v>4</v>
+      </c>
+      <c r="K32" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L32" s="23">
         <v>3.5</v>
       </c>
       <c r="M32" s="13"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="20">
         <v>12</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="41">
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="38">
         <v>40835</v>
       </c>
-      <c r="H33" s="60">
+      <c r="H33" s="38">
         <v>40834</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24">
-        <v>4</v>
-      </c>
-      <c r="K33" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L33" s="24">
+      <c r="I33" s="23">
+        <v>4</v>
+      </c>
+      <c r="J33" s="23">
+        <v>4</v>
+      </c>
+      <c r="K33" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L33" s="23">
         <v>3.5</v>
       </c>
       <c r="M33" s="13"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="20">
         <v>13</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="41">
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="38">
         <v>40830</v>
       </c>
-      <c r="H34" s="60">
+      <c r="H34" s="38">
         <v>40830</v>
       </c>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24">
-        <v>4</v>
-      </c>
-      <c r="K34" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L34" s="24">
+      <c r="I34" s="23">
+        <v>3</v>
+      </c>
+      <c r="J34" s="23">
+        <v>4</v>
+      </c>
+      <c r="K34" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L34" s="23">
         <v>3.5</v>
       </c>
       <c r="M34" s="13"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>14</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="41">
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="38">
         <v>40833</v>
       </c>
-      <c r="H35" s="60">
+      <c r="H35" s="38">
         <v>40833</v>
       </c>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24">
-        <v>4</v>
-      </c>
-      <c r="K35" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L35" s="24">
+      <c r="I35" s="23">
+        <v>3</v>
+      </c>
+      <c r="J35" s="23">
+        <v>4</v>
+      </c>
+      <c r="K35" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L35" s="23">
         <v>3.5</v>
       </c>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>15</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="41">
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="38">
         <v>40834</v>
       </c>
-      <c r="H36" s="60">
+      <c r="H36" s="38">
         <v>40834</v>
       </c>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24">
-        <v>4</v>
-      </c>
-      <c r="K36" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L36" s="24">
+      <c r="I36" s="23">
+        <v>3</v>
+      </c>
+      <c r="J36" s="23">
+        <v>4</v>
+      </c>
+      <c r="K36" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L36" s="23">
         <v>3.5</v>
       </c>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>16</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="41">
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="38">
         <v>40835</v>
       </c>
-      <c r="H37" s="60">
+      <c r="H37" s="38">
         <v>40834</v>
       </c>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24">
-        <v>4</v>
-      </c>
-      <c r="K37" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L37" s="24">
+      <c r="I37" s="23">
+        <v>4</v>
+      </c>
+      <c r="J37" s="23">
+        <v>4</v>
+      </c>
+      <c r="K37" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L37" s="23">
         <v>3.5</v>
       </c>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>17</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="41">
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38">
         <v>40830</v>
       </c>
-      <c r="H38" s="60">
+      <c r="H38" s="38">
         <v>40830</v>
       </c>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24">
-        <v>4</v>
-      </c>
-      <c r="K38" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L38" s="24">
+      <c r="I38" s="23">
+        <v>3</v>
+      </c>
+      <c r="J38" s="23">
+        <v>4</v>
+      </c>
+      <c r="K38" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L38" s="23">
         <v>3.5</v>
       </c>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>18</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="41">
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="38">
         <v>40833</v>
       </c>
-      <c r="H39" s="60">
+      <c r="H39" s="38">
         <v>40832</v>
       </c>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24">
-        <v>4</v>
-      </c>
-      <c r="K39" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L39" s="24">
+      <c r="I39" s="23">
+        <v>4</v>
+      </c>
+      <c r="J39" s="23">
+        <v>4</v>
+      </c>
+      <c r="K39" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L39" s="23">
         <v>3.5</v>
       </c>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>19</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="41">
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="38">
         <v>40834</v>
       </c>
-      <c r="H40" s="60">
+      <c r="H40" s="38">
         <v>40834</v>
       </c>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24">
-        <v>4</v>
-      </c>
-      <c r="K40" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L40" s="24">
+      <c r="I40" s="23">
+        <v>3</v>
+      </c>
+      <c r="J40" s="23">
+        <v>4</v>
+      </c>
+      <c r="K40" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L40" s="23">
         <v>3.5</v>
       </c>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>20</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="41">
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="38">
         <v>40835</v>
       </c>
-      <c r="H41" s="60">
+      <c r="H41" s="38">
         <v>40834</v>
       </c>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24">
-        <v>4</v>
-      </c>
-      <c r="K41" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L41" s="24">
+      <c r="I41" s="23">
+        <v>4</v>
+      </c>
+      <c r="J41" s="23">
+        <v>4</v>
+      </c>
+      <c r="K41" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L41" s="23">
         <v>3.5</v>
       </c>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>21</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="41">
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="38">
         <v>40830</v>
       </c>
-      <c r="H42" s="60">
+      <c r="H42" s="38">
         <v>40830</v>
       </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24">
-        <v>4</v>
-      </c>
-      <c r="K42" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L42" s="24">
+      <c r="I42" s="23">
+        <v>3</v>
+      </c>
+      <c r="J42" s="23">
+        <v>4</v>
+      </c>
+      <c r="K42" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L42" s="23">
         <v>3.5</v>
       </c>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>22</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="41">
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="38">
         <v>40833</v>
       </c>
-      <c r="H43" s="60">
+      <c r="H43" s="38">
         <v>40832</v>
       </c>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24">
-        <v>4</v>
-      </c>
-      <c r="K43" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L43" s="24">
+      <c r="I43" s="23">
+        <v>4</v>
+      </c>
+      <c r="J43" s="23">
+        <v>4</v>
+      </c>
+      <c r="K43" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L43" s="23">
         <v>3.5</v>
       </c>
       <c r="M43" s="13"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>23</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="41">
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="38">
         <v>40834</v>
       </c>
-      <c r="H44" s="60">
+      <c r="H44" s="38">
         <v>40832</v>
       </c>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24">
-        <v>4</v>
-      </c>
-      <c r="K44" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L44" s="24">
+      <c r="I44" s="23">
+        <v>4</v>
+      </c>
+      <c r="J44" s="23">
+        <v>4</v>
+      </c>
+      <c r="K44" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L44" s="23">
         <v>3.5</v>
       </c>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <v>24</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="41">
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="38">
         <v>40835</v>
       </c>
-      <c r="H45" s="60">
+      <c r="H45" s="38">
         <v>40832</v>
       </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24">
-        <v>4</v>
-      </c>
-      <c r="K45" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L45" s="24">
+      <c r="I45" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="J45" s="23">
+        <v>4</v>
+      </c>
+      <c r="K45" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L45" s="23">
         <v>3.5</v>
       </c>
       <c r="M45" s="13"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <v>25</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="41">
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="38">
         <v>40830</v>
       </c>
-      <c r="H46" s="60">
+      <c r="H46" s="38">
         <v>40830</v>
       </c>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24">
-        <v>4</v>
-      </c>
-      <c r="K46" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L46" s="24">
+      <c r="I46" s="23">
+        <v>3</v>
+      </c>
+      <c r="J46" s="23">
+        <v>4</v>
+      </c>
+      <c r="K46" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L46" s="23">
         <v>3.5</v>
       </c>
       <c r="M46" s="13"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>26</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="41">
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="38">
         <v>40833</v>
       </c>
-      <c r="H47" s="60">
+      <c r="H47" s="38">
         <v>40832</v>
       </c>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24">
-        <v>4</v>
-      </c>
-      <c r="K47" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L47" s="24">
+      <c r="I47" s="23">
+        <v>4</v>
+      </c>
+      <c r="J47" s="23">
+        <v>4</v>
+      </c>
+      <c r="K47" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L47" s="23">
         <v>3.5</v>
       </c>
       <c r="M47" s="13"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <v>27</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="41">
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="38">
         <v>40834</v>
       </c>
-      <c r="H48" s="60">
+      <c r="H48" s="38">
         <v>40833</v>
       </c>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24">
-        <v>4</v>
-      </c>
-      <c r="K48" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L48" s="24">
+      <c r="I48" s="23">
+        <v>4</v>
+      </c>
+      <c r="J48" s="23">
+        <v>4</v>
+      </c>
+      <c r="K48" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L48" s="23">
         <v>3.5</v>
       </c>
       <c r="M48" s="13"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>28</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="41">
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="38">
         <v>40835</v>
       </c>
-      <c r="H49" s="60">
+      <c r="H49" s="38">
         <v>40833</v>
       </c>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24">
-        <v>4</v>
-      </c>
-      <c r="K49" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L49" s="24">
+      <c r="I49" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="J49" s="23">
+        <v>4</v>
+      </c>
+      <c r="K49" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L49" s="23">
         <v>3.5</v>
       </c>
       <c r="M49" s="13"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <v>29</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="41">
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="38">
         <v>40830</v>
       </c>
-      <c r="H50" s="60">
+      <c r="H50" s="38">
         <v>40830</v>
       </c>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24">
-        <v>4</v>
-      </c>
-      <c r="K50" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L50" s="24">
+      <c r="I50" s="23">
+        <v>3</v>
+      </c>
+      <c r="J50" s="23">
+        <v>4</v>
+      </c>
+      <c r="K50" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L50" s="23">
         <v>3.5</v>
       </c>
       <c r="M50" s="13"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <v>30</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="41">
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="38">
         <v>40833</v>
       </c>
-      <c r="H51" s="60">
+      <c r="H51" s="38">
         <v>40830</v>
       </c>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24">
-        <v>4</v>
-      </c>
-      <c r="K51" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L51" s="24">
+      <c r="I51" s="23">
+        <v>4</v>
+      </c>
+      <c r="J51" s="23">
+        <v>4</v>
+      </c>
+      <c r="K51" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L51" s="23">
         <v>3.5</v>
       </c>
       <c r="M51" s="13"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <v>31</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="41">
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="38">
         <v>40834</v>
       </c>
-      <c r="H52" s="60">
+      <c r="H52" s="38">
         <v>40830</v>
       </c>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24">
-        <v>4</v>
-      </c>
-      <c r="K52" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L52" s="24">
+      <c r="I52" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="J52" s="23">
+        <v>4</v>
+      </c>
+      <c r="K52" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L52" s="23">
         <v>3.5</v>
       </c>
       <c r="M52" s="13"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <v>32</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C53" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="41">
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="38">
         <v>40835</v>
       </c>
-      <c r="H53" s="60">
+      <c r="H53" s="38">
         <v>40830</v>
       </c>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24">
-        <v>4</v>
-      </c>
-      <c r="K53" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L53" s="24">
+      <c r="I53" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="J53" s="23">
+        <v>4</v>
+      </c>
+      <c r="K53" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L53" s="23">
         <v>3.5</v>
       </c>
       <c r="M53" s="13"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <v>33</v>
       </c>
@@ -3928,26 +3994,30 @@
       <c r="C54" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="41">
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="38">
         <v>40830</v>
       </c>
-      <c r="H54" s="12"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24">
-        <v>4</v>
-      </c>
-      <c r="K54" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L54" s="24">
+      <c r="H54" s="38">
+        <v>40830</v>
+      </c>
+      <c r="I54" s="23">
+        <v>3</v>
+      </c>
+      <c r="J54" s="23">
+        <v>4</v>
+      </c>
+      <c r="K54" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L54" s="23">
         <v>3.5</v>
       </c>
       <c r="M54" s="13"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>34</v>
       </c>
@@ -3957,84 +4027,96 @@
       <c r="C55" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="41">
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="38">
         <v>40833</v>
       </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24">
-        <v>4</v>
-      </c>
-      <c r="K55" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L55" s="24">
+      <c r="H55" s="38">
+        <v>40833</v>
+      </c>
+      <c r="I55" s="23">
+        <v>3</v>
+      </c>
+      <c r="J55" s="23">
+        <v>4</v>
+      </c>
+      <c r="K55" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L55" s="23">
         <v>3.5</v>
       </c>
       <c r="M55" s="13"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>35</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="41">
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="38">
         <v>40834</v>
       </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24">
-        <v>4</v>
-      </c>
-      <c r="K56" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L56" s="24">
+      <c r="H56" s="38">
+        <v>40834</v>
+      </c>
+      <c r="I56" s="23">
+        <v>3</v>
+      </c>
+      <c r="J56" s="23">
+        <v>4</v>
+      </c>
+      <c r="K56" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L56" s="23">
         <v>3.5</v>
       </c>
       <c r="M56" s="13"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>36</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="C57" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="41">
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="38">
         <v>40835</v>
       </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24">
-        <v>4</v>
-      </c>
-      <c r="K57" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L57" s="24">
+      <c r="H57" s="38">
+        <v>40834</v>
+      </c>
+      <c r="I57" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="J57" s="23">
+        <v>4</v>
+      </c>
+      <c r="K57" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L57" s="23">
         <v>3.5</v>
       </c>
       <c r="M57" s="13"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>37</v>
       </c>
@@ -4044,26 +4126,30 @@
       <c r="C58" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="41">
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="38">
         <v>40830</v>
       </c>
-      <c r="H58" s="12"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24">
-        <v>4</v>
-      </c>
-      <c r="K58" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L58" s="24">
+      <c r="H58" s="38">
+        <v>40835</v>
+      </c>
+      <c r="I58" s="23">
+        <v>2</v>
+      </c>
+      <c r="J58" s="23">
+        <v>4</v>
+      </c>
+      <c r="K58" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L58" s="23">
         <v>3.5</v>
       </c>
       <c r="M58" s="13"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>38</v>
       </c>
@@ -4073,191 +4159,205 @@
       <c r="C59" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="41">
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="38">
         <v>40833</v>
       </c>
-      <c r="H59" s="12"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24">
-        <v>4</v>
-      </c>
-      <c r="K59" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L59" s="24">
+      <c r="H59" s="38">
+        <v>40835</v>
+      </c>
+      <c r="I59" s="23">
+        <v>2</v>
+      </c>
+      <c r="J59" s="23">
+        <v>4</v>
+      </c>
+      <c r="K59" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L59" s="23">
         <v>3.5</v>
       </c>
       <c r="M59" s="13"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="20">
         <v>39</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C60" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="41">
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="38">
         <v>40834</v>
       </c>
-      <c r="H60" s="12"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24">
-        <v>4</v>
-      </c>
-      <c r="K60" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L60" s="24">
+      <c r="H60" s="38">
+        <v>40830</v>
+      </c>
+      <c r="I60" s="23">
+        <v>4</v>
+      </c>
+      <c r="J60" s="23">
+        <v>4</v>
+      </c>
+      <c r="K60" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L60" s="23">
         <v>3.5</v>
       </c>
       <c r="M60" s="13"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="20">
         <v>40</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="41">
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="38">
         <v>40835</v>
       </c>
-      <c r="H61" s="12"/>
-      <c r="I61" s="24"/>
-      <c r="J61" s="24">
-        <v>4</v>
-      </c>
-      <c r="K61" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L61" s="24">
+      <c r="H61" s="38">
+        <v>40830</v>
+      </c>
+      <c r="I61" s="23">
+        <v>4</v>
+      </c>
+      <c r="J61" s="23">
+        <v>4</v>
+      </c>
+      <c r="K61" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L61" s="23">
         <v>3.5</v>
       </c>
       <c r="M61" s="13"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="20">
         <v>41</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="34" t="s">
+      <c r="C62" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="41">
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="38">
         <v>40835</v>
       </c>
-      <c r="H62" s="60">
-        <v>40835</v>
-      </c>
-      <c r="I62" s="24"/>
-      <c r="J62" s="24">
+      <c r="H62" s="38">
+        <v>40834</v>
+      </c>
+      <c r="I62" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="J62" s="23">
         <v>5</v>
       </c>
-      <c r="K62" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="L62" s="24">
+      <c r="K62" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="L62" s="23">
         <v>3.5</v>
       </c>
       <c r="M62" s="13"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="20"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="24"/>
-      <c r="J63" s="24"/>
-      <c r="K63" s="24"/>
-      <c r="L63" s="24"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
       <c r="M63" s="13"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="41"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="24"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="24"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
       <c r="M64" s="13"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
       <c r="B65" s="12"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="41"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="24"/>
-      <c r="K65" s="24"/>
-      <c r="L65" s="24"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
       <c r="M65" s="13"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="20"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="24"/>
-      <c r="J66" s="24"/>
-      <c r="K66" s="24"/>
-      <c r="L66" s="24"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
       <c r="M66" s="13"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="21"/>
       <c r="B67" s="14"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
       <c r="M67" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="B20:G21">
+  <autoFilter ref="B20:G62">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>

</xml_diff>

<commit_message>
Danh Gia Cong Viec Tuan 5
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Tuần 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tuần 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tuần 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Tuần 4" sheetId="6" r:id="rId4"/>
+    <sheet name="20111009" sheetId="1" r:id="rId1"/>
+    <sheet name="20111006" sheetId="2" r:id="rId2"/>
+    <sheet name="20111013" sheetId="3" r:id="rId3"/>
+    <sheet name="20111020" sheetId="6" r:id="rId4"/>
+    <sheet name="20111027" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tuần 4'!$B$20:$G$62</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Tuần 4'!$A$1:$M$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20111020'!$B$20:$G$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20111027'!$B$21:$G$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'20111020'!$A$1:$M$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'20111027'!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="110">
   <si>
     <t>Task</t>
   </si>
@@ -274,20 +277,98 @@
   </si>
   <si>
     <t>Xây dựng bố cục project trong thư mục &lt;project_root&gt;/Source</t>
+  </si>
+  <si>
+    <t>ĐÁNH GIÁ CHẤT LƯỢNG LÀM VIỆC TUẦN 5</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
+  </si>
+  <si>
+    <t>Nội dung Review</t>
+  </si>
+  <si>
+    <t>Số lượng Bug</t>
+  </si>
+  <si>
+    <t>Số lượng đã fix</t>
+  </si>
+  <si>
+    <t>Chất lượng file Log</t>
+  </si>
+  <si>
+    <t>HuyDV + ThanhCV + DucNH + LinhTA</t>
+  </si>
+  <si>
+    <t>TuanVA + BaoNDD + TuTM</t>
+  </si>
+  <si>
+    <t>Global Config + Menu Manager  + User Manager + Content Manager</t>
+  </si>
+  <si>
+    <t>Acticle Manager + New &amp; Edit User + Language Manager + Login</t>
+  </si>
+  <si>
+    <t>Media Manager + Media Option + Section Edit + Acticle Edit + Category Edit</t>
+  </si>
+  <si>
+    <t>1. Review Screen Detailed Design</t>
+  </si>
+  <si>
+    <t>2. Code Screen Interface</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình MediaOption + Menu_New</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình SectionManager + CategoryManager + FrontPageManager + ActicleEdit</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình ActicleManager + ActicleCopy + ActicleGlobalConfig</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế layout cho admin module</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình LanguageManager + Login</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình New&amp;EditUser + EditMenuItem</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình Globale Configuration</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình MenuManager + MenuItemManager</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình SectionEdit + ActicleEdit + MoveActicle</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình UserManager + NewMenuItem</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình MediaManager + CopyMenu + MoveMenu</t>
+  </si>
+  <si>
+    <t>ThaoNX + ThiVT + KhoaVT + LinhTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -345,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -709,11 +790,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -798,6 +892,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,6 +942,159 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,6 +1185,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -969,6 +1220,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1144,59 +1396,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="1"/>
-    <col min="3" max="3" width="12.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25">
-      <c r="D1" s="50" t="s">
+    <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="48" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="50"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1209,13 +1461,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="I4" s="45"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="46" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1235,11 +1487,11 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1257,11 +1509,11 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1279,11 +1531,11 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1301,11 +1553,11 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1323,11 +1575,11 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1345,11 +1597,11 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1367,11 +1619,11 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1389,11 +1641,11 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1411,11 +1663,11 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1433,11 +1685,11 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1471,31 +1723,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1503,7 +1755,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1516,34 +1768,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1556,16 +1808,16 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="46" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1587,12 +1839,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1612,12 +1864,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1637,12 +1889,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1662,12 +1914,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1687,12 +1939,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1712,12 +1964,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1737,12 +1989,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1762,12 +2014,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1787,12 +2039,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1812,12 +2064,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1835,7 +2087,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1848,7 +2100,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1861,7 +2113,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1874,7 +2126,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1887,7 +2139,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1900,7 +2152,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1913,7 +2165,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1941,31 +2193,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.875" customWidth="1"/>
-    <col min="8" max="8" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1973,7 +2225,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1986,34 +2238,34 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2026,16 +2278,16 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="46" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2057,12 +2309,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2082,12 +2334,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2107,12 +2359,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2132,12 +2384,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2157,12 +2409,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2182,12 +2434,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2207,12 +2459,12 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2234,12 +2486,12 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2259,12 +2511,12 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2286,12 +2538,12 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2311,7 +2563,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2324,7 +2576,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2337,7 +2589,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2350,7 +2602,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2363,7 +2615,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2376,7 +2628,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2389,7 +2641,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2417,59 +2669,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="E21" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="20" style="6" customWidth="1"/>
-    <col min="4" max="6" width="19.625" style="6" customWidth="1"/>
-    <col min="7" max="12" width="12.125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="28.125" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="6"/>
+    <col min="4" max="6" width="19.5703125" style="6" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.25">
-      <c r="A3" s="53" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
@@ -2486,7 +2738,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1">
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>17</v>
       </c>
@@ -2509,7 +2761,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>1</v>
       </c>
@@ -2539,7 +2791,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>2</v>
       </c>
@@ -2569,7 +2821,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>3</v>
       </c>
@@ -2599,7 +2851,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>4</v>
       </c>
@@ -2629,7 +2881,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>5</v>
       </c>
@@ -2659,7 +2911,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>6</v>
       </c>
@@ -2689,7 +2941,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>7</v>
       </c>
@@ -2719,7 +2971,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>8</v>
       </c>
@@ -2749,7 +3001,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>9</v>
       </c>
@@ -2779,7 +3031,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>10</v>
       </c>
@@ -2809,7 +3061,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>11</v>
       </c>
@@ -2839,7 +3091,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="27"/>
       <c r="C17" s="24"/>
@@ -2854,7 +3106,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2869,49 +3121,49 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="51" t="s">
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="51" t="s">
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="51" t="s">
+      <c r="I20" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51" t="s">
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="9" customFormat="1">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+    <row r="21" spans="1:13" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
       <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
@@ -2924,9 +3176,9 @@
       <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="51"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="M21" s="52"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>1</v>
       </c>
@@ -2959,7 +3211,7 @@
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>2</v>
       </c>
@@ -2992,7 +3244,7 @@
       </c>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>3</v>
       </c>
@@ -3025,7 +3277,7 @@
       </c>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>4</v>
       </c>
@@ -3058,7 +3310,7 @@
       </c>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>5</v>
       </c>
@@ -3091,7 +3343,7 @@
       </c>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>6</v>
       </c>
@@ -3124,7 +3376,7 @@
       </c>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>7</v>
       </c>
@@ -3157,7 +3409,7 @@
       </c>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>8</v>
       </c>
@@ -3190,7 +3442,7 @@
       </c>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>9</v>
       </c>
@@ -3223,7 +3475,7 @@
       </c>
       <c r="M30" s="13"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>10</v>
       </c>
@@ -3256,7 +3508,7 @@
       </c>
       <c r="M31" s="13"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>11</v>
       </c>
@@ -3289,7 +3541,7 @@
       </c>
       <c r="M32" s="13"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="20">
         <v>12</v>
       </c>
@@ -3322,7 +3574,7 @@
       </c>
       <c r="M33" s="13"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="20">
         <v>13</v>
       </c>
@@ -3355,7 +3607,7 @@
       </c>
       <c r="M34" s="13"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>14</v>
       </c>
@@ -3388,7 +3640,7 @@
       </c>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>15</v>
       </c>
@@ -3421,7 +3673,7 @@
       </c>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>16</v>
       </c>
@@ -3454,7 +3706,7 @@
       </c>
       <c r="M37" s="13"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>17</v>
       </c>
@@ -3487,7 +3739,7 @@
       </c>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>18</v>
       </c>
@@ -3520,7 +3772,7 @@
       </c>
       <c r="M39" s="13"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>19</v>
       </c>
@@ -3553,7 +3805,7 @@
       </c>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>20</v>
       </c>
@@ -3586,7 +3838,7 @@
       </c>
       <c r="M41" s="13"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>21</v>
       </c>
@@ -3619,7 +3871,7 @@
       </c>
       <c r="M42" s="13"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>22</v>
       </c>
@@ -3652,7 +3904,7 @@
       </c>
       <c r="M43" s="13"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>23</v>
       </c>
@@ -3685,7 +3937,7 @@
       </c>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <v>24</v>
       </c>
@@ -3718,7 +3970,7 @@
       </c>
       <c r="M45" s="13"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <v>25</v>
       </c>
@@ -3751,7 +4003,7 @@
       </c>
       <c r="M46" s="13"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>26</v>
       </c>
@@ -3784,7 +4036,7 @@
       </c>
       <c r="M47" s="13"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <v>27</v>
       </c>
@@ -3817,7 +4069,7 @@
       </c>
       <c r="M48" s="13"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>28</v>
       </c>
@@ -3850,7 +4102,7 @@
       </c>
       <c r="M49" s="13"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <v>29</v>
       </c>
@@ -3883,7 +4135,7 @@
       </c>
       <c r="M50" s="13"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <v>30</v>
       </c>
@@ -3916,7 +4168,7 @@
       </c>
       <c r="M51" s="13"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <v>31</v>
       </c>
@@ -3949,7 +4201,7 @@
       </c>
       <c r="M52" s="13"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <v>32</v>
       </c>
@@ -3982,7 +4234,7 @@
       </c>
       <c r="M53" s="13"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <v>33</v>
       </c>
@@ -4015,7 +4267,7 @@
       </c>
       <c r="M54" s="13"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>34</v>
       </c>
@@ -4048,7 +4300,7 @@
       </c>
       <c r="M55" s="13"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>35</v>
       </c>
@@ -4081,7 +4333,7 @@
       </c>
       <c r="M56" s="13"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>36</v>
       </c>
@@ -4114,7 +4366,7 @@
       </c>
       <c r="M57" s="13"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>37</v>
       </c>
@@ -4147,7 +4399,7 @@
       </c>
       <c r="M58" s="13"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>38</v>
       </c>
@@ -4180,7 +4432,7 @@
       </c>
       <c r="M59" s="13"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="20">
         <v>39</v>
       </c>
@@ -4213,7 +4465,7 @@
       </c>
       <c r="M60" s="13"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="20">
         <v>40</v>
       </c>
@@ -4246,7 +4498,7 @@
       </c>
       <c r="M61" s="13"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="20">
         <v>41</v>
       </c>
@@ -4279,7 +4531,7 @@
       </c>
       <c r="M62" s="13"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="20"/>
       <c r="B63" s="12"/>
       <c r="C63" s="31"/>
@@ -4294,7 +4546,7 @@
       <c r="L63" s="23"/>
       <c r="M63" s="13"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="12"/>
       <c r="C64" s="31"/>
@@ -4309,7 +4561,7 @@
       <c r="L64" s="23"/>
       <c r="M64" s="13"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
       <c r="B65" s="12"/>
       <c r="C65" s="31"/>
@@ -4324,7 +4576,7 @@
       <c r="L65" s="23"/>
       <c r="M65" s="13"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="20"/>
       <c r="B66" s="12"/>
       <c r="C66" s="31"/>
@@ -4339,7 +4591,7 @@
       <c r="L66" s="23"/>
       <c r="M66" s="13"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="21"/>
       <c r="B67" s="14"/>
       <c r="C67" s="34"/>
@@ -4374,4 +4626,1548 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M68"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="62" customWidth="1"/>
+    <col min="2" max="2" width="30" style="62" customWidth="1"/>
+    <col min="3" max="3" width="20" style="62" customWidth="1"/>
+    <col min="4" max="6" width="19.5703125" style="62" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="62" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="62" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+    </row>
+    <row r="5" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="67">
+        <v>1</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="69">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="69">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="69">
+        <v>3.5</v>
+      </c>
+      <c r="F6" s="69">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="70">
+        <f>AVERAGE(C6:F6)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="71">
+        <v>2</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="73">
+        <v>4</v>
+      </c>
+      <c r="E7" s="73">
+        <v>3</v>
+      </c>
+      <c r="F7" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="74">
+        <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="71">
+        <v>3</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="71">
+        <v>4</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="71">
+        <v>5</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="73">
+        <v>4</v>
+      </c>
+      <c r="E10" s="73">
+        <v>3</v>
+      </c>
+      <c r="F10" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="71">
+        <v>6</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="71">
+        <v>7</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="73">
+        <v>4</v>
+      </c>
+      <c r="E12" s="73">
+        <v>3</v>
+      </c>
+      <c r="F12" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="71">
+        <v>8</v>
+      </c>
+      <c r="B13" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="73">
+        <v>4</v>
+      </c>
+      <c r="E13" s="73">
+        <v>3</v>
+      </c>
+      <c r="F13" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="71">
+        <v>9</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="71">
+        <v>10</v>
+      </c>
+      <c r="B15" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="71">
+        <v>11</v>
+      </c>
+      <c r="B16" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="73">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="74">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="75"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="65"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="82" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="52"/>
+    </row>
+    <row r="23" spans="1:13" s="80" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="83">
+        <v>1</v>
+      </c>
+      <c r="B23" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="86">
+        <v>40837</v>
+      </c>
+      <c r="E23" s="88">
+        <v>40838</v>
+      </c>
+      <c r="F23" s="81">
+        <v>9</v>
+      </c>
+      <c r="G23" s="90">
+        <v>9</v>
+      </c>
+      <c r="H23" s="90">
+        <v>3.75</v>
+      </c>
+      <c r="I23" s="92">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="92">
+        <v>3.5</v>
+      </c>
+      <c r="K23" s="92">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="92">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="93"/>
+    </row>
+    <row r="24" spans="1:13" s="80" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A24" s="84">
+        <v>2</v>
+      </c>
+      <c r="B24" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="87">
+        <v>40837</v>
+      </c>
+      <c r="E24" s="89">
+        <v>40837</v>
+      </c>
+      <c r="F24" s="85">
+        <v>12</v>
+      </c>
+      <c r="G24" s="91">
+        <v>11</v>
+      </c>
+      <c r="H24" s="91">
+        <v>3.75</v>
+      </c>
+      <c r="I24" s="94">
+        <v>3.5</v>
+      </c>
+      <c r="J24" s="94">
+        <v>3.5</v>
+      </c>
+      <c r="K24" s="94">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="94">
+        <v>3.5</v>
+      </c>
+      <c r="M24" s="95"/>
+    </row>
+    <row r="25" spans="1:13" s="80" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A25" s="96">
+        <v>3</v>
+      </c>
+      <c r="B25" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="98">
+        <v>40837</v>
+      </c>
+      <c r="E25" s="99">
+        <v>40837</v>
+      </c>
+      <c r="F25" s="97">
+        <v>51</v>
+      </c>
+      <c r="G25" s="100">
+        <v>31</v>
+      </c>
+      <c r="H25" s="100">
+        <v>3.25</v>
+      </c>
+      <c r="I25" s="101">
+        <v>3</v>
+      </c>
+      <c r="J25" s="101">
+        <v>3.5</v>
+      </c>
+      <c r="K25" s="101">
+        <v>4</v>
+      </c>
+      <c r="L25" s="101">
+        <v>3.5</v>
+      </c>
+      <c r="M25" s="102"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="103"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="103"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="104"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="109" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="107"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="107"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="107"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="A29" s="52"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="M29" s="52"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="67">
+        <v>1</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="37">
+        <v>40844</v>
+      </c>
+      <c r="H30" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="J30" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="K30" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="71">
+        <v>2</v>
+      </c>
+      <c r="B31" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H31" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K31" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L31" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="71">
+        <v>3</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H32" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K32" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="71">
+        <v>4</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H33" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K33" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L33" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="71">
+        <v>5</v>
+      </c>
+      <c r="B34" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H34" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K34" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L34" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="71">
+        <v>6</v>
+      </c>
+      <c r="B35" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H35" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J35" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K35" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L35" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="71">
+        <v>7</v>
+      </c>
+      <c r="B36" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H36" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J36" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K36" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L36" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="71">
+        <v>8</v>
+      </c>
+      <c r="B37" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H37" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J37" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K37" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="71">
+        <v>9</v>
+      </c>
+      <c r="B38" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H38" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J38" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K38" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="71">
+        <v>10</v>
+      </c>
+      <c r="B39" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H39" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I39" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J39" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K39" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L39" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="71">
+        <v>11</v>
+      </c>
+      <c r="B40" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="L40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="20"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="20"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="20"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="13"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="13"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="13"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="13"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="106"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="107"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="106"/>
+      <c r="J51" s="106"/>
+      <c r="K51" s="106"/>
+      <c r="L51" s="106"/>
+      <c r="M51" s="107"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="106"/>
+      <c r="B52" s="107"/>
+      <c r="C52" s="107"/>
+      <c r="D52" s="107"/>
+      <c r="E52" s="107"/>
+      <c r="F52" s="107"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="108"/>
+      <c r="I52" s="106"/>
+      <c r="J52" s="106"/>
+      <c r="K52" s="106"/>
+      <c r="L52" s="106"/>
+      <c r="M52" s="107"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="106"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="107"/>
+      <c r="D53" s="107"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="107"/>
+      <c r="G53" s="108"/>
+      <c r="H53" s="108"/>
+      <c r="I53" s="106"/>
+      <c r="J53" s="106"/>
+      <c r="K53" s="106"/>
+      <c r="L53" s="106"/>
+      <c r="M53" s="107"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="106"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="107"/>
+      <c r="D54" s="107"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="107"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="106"/>
+      <c r="J54" s="106"/>
+      <c r="K54" s="106"/>
+      <c r="L54" s="106"/>
+      <c r="M54" s="107"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="106"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="107"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="107"/>
+      <c r="G55" s="108"/>
+      <c r="H55" s="108"/>
+      <c r="I55" s="106"/>
+      <c r="J55" s="106"/>
+      <c r="K55" s="106"/>
+      <c r="L55" s="106"/>
+      <c r="M55" s="107"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="106"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="108"/>
+      <c r="H56" s="108"/>
+      <c r="I56" s="106"/>
+      <c r="J56" s="106"/>
+      <c r="K56" s="106"/>
+      <c r="L56" s="106"/>
+      <c r="M56" s="107"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="106"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="107"/>
+      <c r="D57" s="107"/>
+      <c r="E57" s="107"/>
+      <c r="F57" s="107"/>
+      <c r="G57" s="108"/>
+      <c r="H57" s="108"/>
+      <c r="I57" s="106"/>
+      <c r="J57" s="106"/>
+      <c r="K57" s="106"/>
+      <c r="L57" s="106"/>
+      <c r="M57" s="107"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="106"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="107"/>
+      <c r="D58" s="107"/>
+      <c r="E58" s="107"/>
+      <c r="F58" s="107"/>
+      <c r="G58" s="108"/>
+      <c r="H58" s="108"/>
+      <c r="I58" s="106"/>
+      <c r="J58" s="106"/>
+      <c r="K58" s="106"/>
+      <c r="L58" s="106"/>
+      <c r="M58" s="107"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="106"/>
+      <c r="B59" s="107"/>
+      <c r="C59" s="107"/>
+      <c r="D59" s="107"/>
+      <c r="E59" s="107"/>
+      <c r="F59" s="107"/>
+      <c r="G59" s="108"/>
+      <c r="H59" s="108"/>
+      <c r="I59" s="106"/>
+      <c r="J59" s="106"/>
+      <c r="K59" s="106"/>
+      <c r="L59" s="106"/>
+      <c r="M59" s="107"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="106"/>
+      <c r="B60" s="107"/>
+      <c r="C60" s="107"/>
+      <c r="D60" s="107"/>
+      <c r="E60" s="107"/>
+      <c r="F60" s="107"/>
+      <c r="G60" s="108"/>
+      <c r="H60" s="108"/>
+      <c r="I60" s="106"/>
+      <c r="J60" s="106"/>
+      <c r="K60" s="106"/>
+      <c r="L60" s="106"/>
+      <c r="M60" s="107"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="106"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="107"/>
+      <c r="D61" s="107"/>
+      <c r="E61" s="107"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="108"/>
+      <c r="H61" s="108"/>
+      <c r="I61" s="106"/>
+      <c r="J61" s="106"/>
+      <c r="K61" s="106"/>
+      <c r="L61" s="106"/>
+      <c r="M61" s="107"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="106"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="107"/>
+      <c r="D62" s="107"/>
+      <c r="E62" s="107"/>
+      <c r="F62" s="107"/>
+      <c r="G62" s="108"/>
+      <c r="H62" s="108"/>
+      <c r="I62" s="106"/>
+      <c r="J62" s="106"/>
+      <c r="K62" s="106"/>
+      <c r="L62" s="106"/>
+      <c r="M62" s="107"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="106"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="107"/>
+      <c r="D63" s="107"/>
+      <c r="E63" s="107"/>
+      <c r="F63" s="107"/>
+      <c r="G63" s="108"/>
+      <c r="H63" s="108"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="106"/>
+      <c r="K63" s="106"/>
+      <c r="L63" s="106"/>
+      <c r="M63" s="107"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="106"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="107"/>
+      <c r="D64" s="107"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="107"/>
+      <c r="G64" s="108"/>
+      <c r="H64" s="108"/>
+      <c r="I64" s="106"/>
+      <c r="J64" s="106"/>
+      <c r="K64" s="106"/>
+      <c r="L64" s="106"/>
+      <c r="M64" s="107"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="106"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="107"/>
+      <c r="D65" s="107"/>
+      <c r="E65" s="107"/>
+      <c r="F65" s="107"/>
+      <c r="G65" s="108"/>
+      <c r="H65" s="108"/>
+      <c r="I65" s="106"/>
+      <c r="J65" s="106"/>
+      <c r="K65" s="106"/>
+      <c r="L65" s="106"/>
+      <c r="M65" s="107"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="106"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="107"/>
+      <c r="D66" s="107"/>
+      <c r="E66" s="107"/>
+      <c r="F66" s="107"/>
+      <c r="G66" s="108"/>
+      <c r="H66" s="108"/>
+      <c r="I66" s="106"/>
+      <c r="J66" s="106"/>
+      <c r="K66" s="106"/>
+      <c r="L66" s="106"/>
+      <c r="M66" s="107"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="106"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="107"/>
+      <c r="D67" s="107"/>
+      <c r="E67" s="107"/>
+      <c r="F67" s="107"/>
+      <c r="G67" s="108"/>
+      <c r="H67" s="108"/>
+      <c r="I67" s="106"/>
+      <c r="J67" s="106"/>
+      <c r="K67" s="106"/>
+      <c r="L67" s="106"/>
+      <c r="M67" s="107"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="106"/>
+      <c r="B68" s="107"/>
+      <c r="C68" s="107"/>
+      <c r="D68" s="107"/>
+      <c r="E68" s="107"/>
+      <c r="F68" s="107"/>
+      <c r="G68" s="108"/>
+      <c r="H68" s="108"/>
+      <c r="I68" s="106"/>
+      <c r="J68" s="106"/>
+      <c r="K68" s="106"/>
+      <c r="L68" s="106"/>
+      <c r="M68" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:F29"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="F21:F22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật tổng hợp đánh giá và project plan.
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -339,9 +339,6 @@
     <t>Nghiên cứu Zend Form và thiết kế màn hình New&amp;EditUser + EditMenuItem</t>
   </si>
   <si>
-    <t>Nghiên cứu Zend Form và thiết kế màn hình Globale Configuration</t>
-  </si>
-  <si>
     <t>Nghiên cứu Zend Form và thiết kế màn hình MenuManager + MenuItemManager</t>
   </si>
   <si>
@@ -354,7 +351,10 @@
     <t>Nghiên cứu Zend Form và thiết kế màn hình MediaManager + CopyMenu + MoveMenu</t>
   </si>
   <si>
-    <t>ThaoNX + ThiVT + KhoaVT + LinhTA</t>
+    <t>ThaoNX + ThiVT + KhoaVT + DungDV</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Zend Form và thiết kế màn hình Global Configuration</t>
   </si>
 </sst>
 </file>
@@ -895,6 +895,153 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -946,155 +1093,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,39 +1416,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="51"/>
+      <c r="E1" s="100"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="50"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1461,13 +1461,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="45"/>
+      <c r="I4" s="94"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="95" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1491,7 +1491,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="96"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1513,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1579,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1601,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1645,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="47"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="96"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1689,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1744,10 +1744,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="51"/>
+      <c r="E1" s="100"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1770,22 +1770,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -1793,9 +1793,9 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="45"/>
+      <c r="I4" s="94"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -1817,7 +1817,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="95" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1844,7 +1844,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="96"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1894,7 +1894,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1944,7 +1944,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1994,7 +1994,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="47"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="96"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2214,10 +2214,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="51"/>
+      <c r="E1" s="100"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2240,22 +2240,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -2263,9 +2263,9 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="45"/>
+      <c r="I4" s="94"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -2287,7 +2287,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="95" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2314,7 +2314,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="96"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2339,7 +2339,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="47"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="47"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="47"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="47"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="96"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2688,38 +2688,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
@@ -3127,43 +3127,43 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="52" t="s">
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="52" t="s">
+      <c r="H20" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="52" t="s">
+      <c r="I20" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52" t="s">
+      <c r="J20" s="101"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="101" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
+      <c r="A21" s="101"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
       <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
@@ -3176,7 +3176,7 @@
       <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="52"/>
+      <c r="M21" s="101"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
@@ -4632,521 +4632,521 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="62" customWidth="1"/>
-    <col min="2" max="2" width="30" style="62" customWidth="1"/>
-    <col min="3" max="3" width="20" style="62" customWidth="1"/>
-    <col min="4" max="6" width="19.5703125" style="62" customWidth="1"/>
-    <col min="7" max="12" width="12.140625" style="62" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" style="62" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="4.42578125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="30" style="45" customWidth="1"/>
+    <col min="3" max="3" width="20" style="45" customWidth="1"/>
+    <col min="4" max="6" width="19.5703125" style="45" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="45" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="45" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="110" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-    </row>
-    <row r="5" spans="1:13" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+    </row>
+    <row r="5" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" s="48" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="67">
+      <c r="A6" s="49">
         <v>1</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="69">
-        <v>3.5</v>
-      </c>
-      <c r="D6" s="69">
-        <v>3.5</v>
-      </c>
-      <c r="E6" s="69">
-        <v>3.5</v>
-      </c>
-      <c r="F6" s="69">
-        <v>3.5</v>
-      </c>
-      <c r="G6" s="70">
+      <c r="C6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="F6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="52">
         <f>AVERAGE(C6:F6)</f>
         <v>3.5</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="71">
+      <c r="A7" s="53">
         <v>2</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D7" s="73">
-        <v>4</v>
-      </c>
-      <c r="E7" s="73">
+      <c r="C7" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="55">
+        <v>4</v>
+      </c>
+      <c r="E7" s="55">
         <v>3</v>
       </c>
-      <c r="F7" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G7" s="74">
+      <c r="F7" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="56">
         <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
         <v>3.5</v>
       </c>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="71">
+      <c r="A8" s="53">
         <v>3</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D8" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E8" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F8" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G8" s="74">
+      <c r="C8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="71">
-        <v>4</v>
-      </c>
-      <c r="B9" s="72" t="s">
+      <c r="A9" s="53">
+        <v>4</v>
+      </c>
+      <c r="B9" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G9" s="74">
+      <c r="C9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="71">
+      <c r="A10" s="53">
         <v>5</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D10" s="73">
-        <v>4</v>
-      </c>
-      <c r="E10" s="73">
+      <c r="C10" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="55">
+        <v>4</v>
+      </c>
+      <c r="E10" s="55">
         <v>3</v>
       </c>
-      <c r="F10" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G10" s="74">
+      <c r="F10" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="71">
+      <c r="A11" s="53">
         <v>6</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D11" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E11" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G11" s="74">
+      <c r="C11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="71">
+      <c r="A12" s="53">
         <v>7</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="73">
-        <v>4</v>
-      </c>
-      <c r="E12" s="73">
+      <c r="C12" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="55">
+        <v>4</v>
+      </c>
+      <c r="E12" s="55">
         <v>3</v>
       </c>
-      <c r="F12" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G12" s="74">
+      <c r="F12" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="71">
+      <c r="A13" s="53">
         <v>8</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D13" s="73">
-        <v>4</v>
-      </c>
-      <c r="E13" s="73">
+      <c r="C13" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="55">
+        <v>4</v>
+      </c>
+      <c r="E13" s="55">
         <v>3</v>
       </c>
-      <c r="F13" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G13" s="74">
+      <c r="F13" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="71">
+      <c r="A14" s="53">
         <v>9</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D14" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E14" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G14" s="74">
+      <c r="C14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="71">
+      <c r="A15" s="53">
         <v>10</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D15" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E15" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F15" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G15" s="74">
+      <c r="C15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="71">
+      <c r="A16" s="53">
         <v>11</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="D16" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="E16" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="F16" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="G16" s="74">
+      <c r="C16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="56">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="61" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="52" t="s">
+      <c r="D21" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="52" t="s">
+      <c r="F21" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="52" t="s">
+      <c r="G21" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="52" t="s">
+      <c r="H21" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52" t="s">
+      <c r="J21" s="101"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="101" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="82" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
+    <row r="22" spans="1:13" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="101"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="101"/>
       <c r="I22" s="44" t="s">
         <v>34</v>
       </c>
@@ -5159,195 +5159,195 @@
       <c r="L22" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="52"/>
-    </row>
-    <row r="23" spans="1:13" s="80" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83">
+      <c r="M22" s="101"/>
+    </row>
+    <row r="23" spans="1:13" s="62" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="65">
         <v>1</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="86">
+      <c r="D23" s="68">
         <v>40837</v>
       </c>
-      <c r="E23" s="88">
+      <c r="E23" s="70">
         <v>40838</v>
       </c>
-      <c r="F23" s="81">
+      <c r="F23" s="63">
         <v>9</v>
       </c>
-      <c r="G23" s="90">
+      <c r="G23" s="72">
         <v>9</v>
       </c>
-      <c r="H23" s="90">
+      <c r="H23" s="72">
         <v>3.75</v>
       </c>
-      <c r="I23" s="92">
-        <v>3.5</v>
-      </c>
-      <c r="J23" s="92">
-        <v>3.5</v>
-      </c>
-      <c r="K23" s="92">
-        <v>3.5</v>
-      </c>
-      <c r="L23" s="92">
-        <v>3.5</v>
-      </c>
-      <c r="M23" s="93"/>
-    </row>
-    <row r="24" spans="1:13" s="80" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A24" s="84">
+      <c r="I23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="K23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="75"/>
+    </row>
+    <row r="24" spans="1:13" s="62" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A24" s="66">
         <v>2</v>
       </c>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="87">
+      <c r="D24" s="69">
         <v>40837</v>
       </c>
-      <c r="E24" s="89">
+      <c r="E24" s="71">
         <v>40837</v>
       </c>
-      <c r="F24" s="85">
+      <c r="F24" s="67">
         <v>12</v>
       </c>
-      <c r="G24" s="91">
+      <c r="G24" s="73">
         <v>11</v>
       </c>
-      <c r="H24" s="91">
+      <c r="H24" s="73">
         <v>3.75</v>
       </c>
-      <c r="I24" s="94">
-        <v>3.5</v>
-      </c>
-      <c r="J24" s="94">
-        <v>3.5</v>
-      </c>
-      <c r="K24" s="94">
-        <v>3.5</v>
-      </c>
-      <c r="L24" s="94">
-        <v>3.5</v>
-      </c>
-      <c r="M24" s="95"/>
-    </row>
-    <row r="25" spans="1:13" s="80" customFormat="1" ht="48" x14ac:dyDescent="0.25">
-      <c r="A25" s="96">
+      <c r="I24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="J24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="K24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="M24" s="77"/>
+    </row>
+    <row r="25" spans="1:13" s="62" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A25" s="78">
         <v>3</v>
       </c>
-      <c r="B25" s="97" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="97" t="s">
+      <c r="B25" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="98">
+      <c r="D25" s="80">
         <v>40837</v>
       </c>
-      <c r="E25" s="99">
+      <c r="E25" s="81">
         <v>40837</v>
       </c>
-      <c r="F25" s="97">
+      <c r="F25" s="79">
         <v>51</v>
       </c>
-      <c r="G25" s="100">
+      <c r="G25" s="82">
         <v>31</v>
       </c>
-      <c r="H25" s="100">
+      <c r="H25" s="82">
         <v>3.25</v>
       </c>
-      <c r="I25" s="101">
+      <c r="I25" s="83">
         <v>3</v>
       </c>
-      <c r="J25" s="101">
-        <v>3.5</v>
-      </c>
-      <c r="K25" s="101">
-        <v>4</v>
-      </c>
-      <c r="L25" s="101">
-        <v>3.5</v>
-      </c>
-      <c r="M25" s="102"/>
+      <c r="J25" s="83">
+        <v>3.5</v>
+      </c>
+      <c r="K25" s="83">
+        <v>4</v>
+      </c>
+      <c r="L25" s="83">
+        <v>3.5</v>
+      </c>
+      <c r="M25" s="84"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
-      <c r="B26" s="104"/>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="104"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="103"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="104"/>
+      <c r="A26" s="85"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="86"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="109" t="s">
+      <c r="A27" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="107"/>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="107"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="52" t="s">
+      <c r="D28" s="105"/>
+      <c r="E28" s="105"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="H28" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="52" t="s">
+      <c r="I28" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52" t="s">
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
+      <c r="A29" s="101"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
       <c r="I29" s="44" t="s">
         <v>34</v>
       </c>
@@ -5360,13 +5360,13 @@
       <c r="L29" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="52"/>
+      <c r="M29" s="101"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="67">
+      <c r="A30" s="49">
         <v>1</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="50" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="28" t="s">
@@ -5378,28 +5378,28 @@
       <c r="G30" s="37">
         <v>40844</v>
       </c>
-      <c r="H30" s="110" t="s">
+      <c r="H30" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="I30" s="110" t="s">
+      <c r="I30" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="J30" s="110" t="s">
+      <c r="J30" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="K30" s="110" t="s">
+      <c r="K30" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="L30" s="110" t="s">
+      <c r="L30" s="92" t="s">
         <v>97</v>
       </c>
       <c r="M30" s="11"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="71">
+      <c r="A31" s="53">
         <v>2</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="54" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="31" t="s">
@@ -5411,28 +5411,28 @@
       <c r="G31" s="38">
         <v>40844</v>
       </c>
-      <c r="H31" s="111" t="s">
+      <c r="H31" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I31" s="111" t="s">
+      <c r="I31" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="111" t="s">
+      <c r="J31" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K31" s="111" t="s">
+      <c r="K31" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L31" s="111" t="s">
+      <c r="L31" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="71">
+      <c r="A32" s="53">
         <v>3</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="54" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="31" t="s">
@@ -5444,28 +5444,28 @@
       <c r="G32" s="38">
         <v>40844</v>
       </c>
-      <c r="H32" s="111" t="s">
+      <c r="H32" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I32" s="111" t="s">
+      <c r="I32" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J32" s="111" t="s">
+      <c r="J32" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K32" s="111" t="s">
+      <c r="K32" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L32" s="111" t="s">
+      <c r="L32" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="71">
-        <v>4</v>
-      </c>
-      <c r="B33" s="72" t="s">
+      <c r="A33" s="53">
+        <v>4</v>
+      </c>
+      <c r="B33" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="31" t="s">
@@ -5477,28 +5477,28 @@
       <c r="G33" s="38">
         <v>40844</v>
       </c>
-      <c r="H33" s="111" t="s">
+      <c r="H33" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="111" t="s">
+      <c r="I33" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J33" s="111" t="s">
+      <c r="J33" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K33" s="111" t="s">
+      <c r="K33" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="111" t="s">
+      <c r="L33" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M33" s="13"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="71">
+      <c r="A34" s="53">
         <v>5</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="54" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="31" t="s">
@@ -5510,28 +5510,28 @@
       <c r="G34" s="38">
         <v>40844</v>
       </c>
-      <c r="H34" s="111" t="s">
+      <c r="H34" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="111" t="s">
+      <c r="I34" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="111" t="s">
+      <c r="J34" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K34" s="111" t="s">
+      <c r="K34" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L34" s="111" t="s">
+      <c r="L34" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M34" s="13"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="71">
+      <c r="A35" s="53">
         <v>6</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="54" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="31" t="s">
@@ -5543,32 +5543,32 @@
       <c r="G35" s="38">
         <v>40844</v>
       </c>
-      <c r="H35" s="111" t="s">
+      <c r="H35" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I35" s="111" t="s">
+      <c r="I35" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J35" s="111" t="s">
+      <c r="J35" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K35" s="111" t="s">
+      <c r="K35" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L35" s="111" t="s">
+      <c r="L35" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M35" s="13"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="71">
+      <c r="A36" s="53">
         <v>7</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="54" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="32"/>
@@ -5576,32 +5576,32 @@
       <c r="G36" s="38">
         <v>40844</v>
       </c>
-      <c r="H36" s="111" t="s">
+      <c r="H36" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I36" s="111" t="s">
+      <c r="I36" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J36" s="111" t="s">
+      <c r="J36" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K36" s="111" t="s">
+      <c r="K36" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L36" s="111" t="s">
+      <c r="L36" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="71">
+      <c r="A37" s="53">
         <v>8</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="32"/>
@@ -5609,32 +5609,32 @@
       <c r="G37" s="38">
         <v>40844</v>
       </c>
-      <c r="H37" s="111" t="s">
+      <c r="H37" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I37" s="111" t="s">
+      <c r="I37" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J37" s="111" t="s">
+      <c r="J37" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K37" s="111" t="s">
+      <c r="K37" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L37" s="111" t="s">
+      <c r="L37" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="71">
+      <c r="A38" s="53">
         <v>9</v>
       </c>
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
@@ -5642,32 +5642,32 @@
       <c r="G38" s="38">
         <v>40844</v>
       </c>
-      <c r="H38" s="111" t="s">
+      <c r="H38" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I38" s="111" t="s">
+      <c r="I38" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J38" s="111" t="s">
+      <c r="J38" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K38" s="111" t="s">
+      <c r="K38" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L38" s="111" t="s">
+      <c r="L38" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M38" s="13"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="71">
+      <c r="A39" s="53">
         <v>10</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="54" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="32"/>
@@ -5675,32 +5675,32 @@
       <c r="G39" s="38">
         <v>40844</v>
       </c>
-      <c r="H39" s="111" t="s">
+      <c r="H39" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I39" s="111" t="s">
+      <c r="I39" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J39" s="111" t="s">
+      <c r="J39" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="111" t="s">
+      <c r="K39" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L39" s="111" t="s">
+      <c r="L39" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M39" s="13"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="71">
+      <c r="A40" s="53">
         <v>11</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="54" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
@@ -5708,19 +5708,19 @@
       <c r="G40" s="38">
         <v>40844</v>
       </c>
-      <c r="H40" s="111" t="s">
+      <c r="H40" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="I40" s="111" t="s">
+      <c r="I40" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="J40" s="111" t="s">
+      <c r="J40" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="111" t="s">
+      <c r="K40" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="L40" s="111" t="s">
+      <c r="L40" s="93" t="s">
         <v>97</v>
       </c>
       <c r="M40" s="13"/>
@@ -5876,287 +5876,277 @@
       <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="106"/>
-      <c r="B51" s="107"/>
-      <c r="C51" s="107"/>
-      <c r="D51" s="107"/>
-      <c r="E51" s="107"/>
-      <c r="F51" s="107"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="108"/>
-      <c r="I51" s="106"/>
-      <c r="J51" s="106"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="107"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="88"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="88"/>
+      <c r="M51" s="89"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="106"/>
-      <c r="B52" s="107"/>
-      <c r="C52" s="107"/>
-      <c r="D52" s="107"/>
-      <c r="E52" s="107"/>
-      <c r="F52" s="107"/>
-      <c r="G52" s="108"/>
-      <c r="H52" s="108"/>
-      <c r="I52" s="106"/>
-      <c r="J52" s="106"/>
-      <c r="K52" s="106"/>
-      <c r="L52" s="106"/>
-      <c r="M52" s="107"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
+      <c r="K52" s="88"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="89"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="106"/>
-      <c r="B53" s="107"/>
-      <c r="C53" s="107"/>
-      <c r="D53" s="107"/>
-      <c r="E53" s="107"/>
-      <c r="F53" s="107"/>
-      <c r="G53" s="108"/>
-      <c r="H53" s="108"/>
-      <c r="I53" s="106"/>
-      <c r="J53" s="106"/>
-      <c r="K53" s="106"/>
-      <c r="L53" s="106"/>
-      <c r="M53" s="107"/>
+      <c r="A53" s="88"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="90"/>
+      <c r="I53" s="88"/>
+      <c r="J53" s="88"/>
+      <c r="K53" s="88"/>
+      <c r="L53" s="88"/>
+      <c r="M53" s="89"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="106"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="107"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="107"/>
-      <c r="F54" s="107"/>
-      <c r="G54" s="108"/>
-      <c r="H54" s="108"/>
-      <c r="I54" s="106"/>
-      <c r="J54" s="106"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="107"/>
+      <c r="A54" s="88"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="90"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="88"/>
+      <c r="K54" s="88"/>
+      <c r="L54" s="88"/>
+      <c r="M54" s="89"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="106"/>
-      <c r="B55" s="107"/>
-      <c r="C55" s="107"/>
-      <c r="D55" s="107"/>
-      <c r="E55" s="107"/>
-      <c r="F55" s="107"/>
-      <c r="G55" s="108"/>
-      <c r="H55" s="108"/>
-      <c r="I55" s="106"/>
-      <c r="J55" s="106"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="107"/>
+      <c r="A55" s="88"/>
+      <c r="B55" s="89"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="89"/>
+      <c r="G55" s="90"/>
+      <c r="H55" s="90"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="88"/>
+      <c r="M55" s="89"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="106"/>
-      <c r="B56" s="107"/>
-      <c r="C56" s="107"/>
-      <c r="D56" s="107"/>
-      <c r="E56" s="107"/>
-      <c r="F56" s="107"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="108"/>
-      <c r="I56" s="106"/>
-      <c r="J56" s="106"/>
-      <c r="K56" s="106"/>
-      <c r="L56" s="106"/>
-      <c r="M56" s="107"/>
+      <c r="A56" s="88"/>
+      <c r="B56" s="89"/>
+      <c r="C56" s="89"/>
+      <c r="D56" s="89"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="89"/>
+      <c r="G56" s="90"/>
+      <c r="H56" s="90"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="88"/>
+      <c r="M56" s="89"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="106"/>
-      <c r="B57" s="107"/>
-      <c r="C57" s="107"/>
-      <c r="D57" s="107"/>
-      <c r="E57" s="107"/>
-      <c r="F57" s="107"/>
-      <c r="G57" s="108"/>
-      <c r="H57" s="108"/>
-      <c r="I57" s="106"/>
-      <c r="J57" s="106"/>
-      <c r="K57" s="106"/>
-      <c r="L57" s="106"/>
-      <c r="M57" s="107"/>
+      <c r="A57" s="88"/>
+      <c r="B57" s="89"/>
+      <c r="C57" s="89"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="89"/>
+      <c r="G57" s="90"/>
+      <c r="H57" s="90"/>
+      <c r="I57" s="88"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="88"/>
+      <c r="M57" s="89"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="106"/>
-      <c r="B58" s="107"/>
-      <c r="C58" s="107"/>
-      <c r="D58" s="107"/>
-      <c r="E58" s="107"/>
-      <c r="F58" s="107"/>
-      <c r="G58" s="108"/>
-      <c r="H58" s="108"/>
-      <c r="I58" s="106"/>
-      <c r="J58" s="106"/>
-      <c r="K58" s="106"/>
-      <c r="L58" s="106"/>
-      <c r="M58" s="107"/>
+      <c r="A58" s="88"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="89"/>
+      <c r="G58" s="90"/>
+      <c r="H58" s="90"/>
+      <c r="I58" s="88"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="88"/>
+      <c r="L58" s="88"/>
+      <c r="M58" s="89"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="106"/>
-      <c r="B59" s="107"/>
-      <c r="C59" s="107"/>
-      <c r="D59" s="107"/>
-      <c r="E59" s="107"/>
-      <c r="F59" s="107"/>
-      <c r="G59" s="108"/>
-      <c r="H59" s="108"/>
-      <c r="I59" s="106"/>
-      <c r="J59" s="106"/>
-      <c r="K59" s="106"/>
-      <c r="L59" s="106"/>
-      <c r="M59" s="107"/>
+      <c r="A59" s="88"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="90"/>
+      <c r="H59" s="90"/>
+      <c r="I59" s="88"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="88"/>
+      <c r="M59" s="89"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="106"/>
-      <c r="B60" s="107"/>
-      <c r="C60" s="107"/>
-      <c r="D60" s="107"/>
-      <c r="E60" s="107"/>
-      <c r="F60" s="107"/>
-      <c r="G60" s="108"/>
-      <c r="H60" s="108"/>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="107"/>
+      <c r="A60" s="88"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="89"/>
+      <c r="D60" s="89"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="89"/>
+      <c r="G60" s="90"/>
+      <c r="H60" s="90"/>
+      <c r="I60" s="88"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="88"/>
+      <c r="L60" s="88"/>
+      <c r="M60" s="89"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="106"/>
-      <c r="B61" s="107"/>
-      <c r="C61" s="107"/>
-      <c r="D61" s="107"/>
-      <c r="E61" s="107"/>
-      <c r="F61" s="107"/>
-      <c r="G61" s="108"/>
-      <c r="H61" s="108"/>
-      <c r="I61" s="106"/>
-      <c r="J61" s="106"/>
-      <c r="K61" s="106"/>
-      <c r="L61" s="106"/>
-      <c r="M61" s="107"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="89"/>
+      <c r="D61" s="89"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="89"/>
+      <c r="G61" s="90"/>
+      <c r="H61" s="90"/>
+      <c r="I61" s="88"/>
+      <c r="J61" s="88"/>
+      <c r="K61" s="88"/>
+      <c r="L61" s="88"/>
+      <c r="M61" s="89"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="106"/>
-      <c r="B62" s="107"/>
-      <c r="C62" s="107"/>
-      <c r="D62" s="107"/>
-      <c r="E62" s="107"/>
-      <c r="F62" s="107"/>
-      <c r="G62" s="108"/>
-      <c r="H62" s="108"/>
-      <c r="I62" s="106"/>
-      <c r="J62" s="106"/>
-      <c r="K62" s="106"/>
-      <c r="L62" s="106"/>
-      <c r="M62" s="107"/>
+      <c r="A62" s="88"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="89"/>
+      <c r="D62" s="89"/>
+      <c r="E62" s="89"/>
+      <c r="F62" s="89"/>
+      <c r="G62" s="90"/>
+      <c r="H62" s="90"/>
+      <c r="I62" s="88"/>
+      <c r="J62" s="88"/>
+      <c r="K62" s="88"/>
+      <c r="L62" s="88"/>
+      <c r="M62" s="89"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="106"/>
-      <c r="B63" s="107"/>
-      <c r="C63" s="107"/>
-      <c r="D63" s="107"/>
-      <c r="E63" s="107"/>
-      <c r="F63" s="107"/>
-      <c r="G63" s="108"/>
-      <c r="H63" s="108"/>
-      <c r="I63" s="106"/>
-      <c r="J63" s="106"/>
-      <c r="K63" s="106"/>
-      <c r="L63" s="106"/>
-      <c r="M63" s="107"/>
+      <c r="A63" s="88"/>
+      <c r="B63" s="89"/>
+      <c r="C63" s="89"/>
+      <c r="D63" s="89"/>
+      <c r="E63" s="89"/>
+      <c r="F63" s="89"/>
+      <c r="G63" s="90"/>
+      <c r="H63" s="90"/>
+      <c r="I63" s="88"/>
+      <c r="J63" s="88"/>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
+      <c r="M63" s="89"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="106"/>
-      <c r="B64" s="107"/>
-      <c r="C64" s="107"/>
-      <c r="D64" s="107"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="107"/>
-      <c r="G64" s="108"/>
-      <c r="H64" s="108"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="106"/>
-      <c r="K64" s="106"/>
-      <c r="L64" s="106"/>
-      <c r="M64" s="107"/>
+      <c r="A64" s="88"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="90"/>
+      <c r="H64" s="90"/>
+      <c r="I64" s="88"/>
+      <c r="J64" s="88"/>
+      <c r="K64" s="88"/>
+      <c r="L64" s="88"/>
+      <c r="M64" s="89"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="106"/>
-      <c r="B65" s="107"/>
-      <c r="C65" s="107"/>
-      <c r="D65" s="107"/>
-      <c r="E65" s="107"/>
-      <c r="F65" s="107"/>
-      <c r="G65" s="108"/>
-      <c r="H65" s="108"/>
-      <c r="I65" s="106"/>
-      <c r="J65" s="106"/>
-      <c r="K65" s="106"/>
-      <c r="L65" s="106"/>
-      <c r="M65" s="107"/>
+      <c r="A65" s="88"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="89"/>
+      <c r="E65" s="89"/>
+      <c r="F65" s="89"/>
+      <c r="G65" s="90"/>
+      <c r="H65" s="90"/>
+      <c r="I65" s="88"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="88"/>
+      <c r="L65" s="88"/>
+      <c r="M65" s="89"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="106"/>
-      <c r="B66" s="107"/>
-      <c r="C66" s="107"/>
-      <c r="D66" s="107"/>
-      <c r="E66" s="107"/>
-      <c r="F66" s="107"/>
-      <c r="G66" s="108"/>
-      <c r="H66" s="108"/>
-      <c r="I66" s="106"/>
-      <c r="J66" s="106"/>
-      <c r="K66" s="106"/>
-      <c r="L66" s="106"/>
-      <c r="M66" s="107"/>
+      <c r="A66" s="88"/>
+      <c r="B66" s="89"/>
+      <c r="C66" s="89"/>
+      <c r="D66" s="89"/>
+      <c r="E66" s="89"/>
+      <c r="F66" s="89"/>
+      <c r="G66" s="90"/>
+      <c r="H66" s="90"/>
+      <c r="I66" s="88"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="88"/>
+      <c r="M66" s="89"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="106"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="107"/>
-      <c r="D67" s="107"/>
-      <c r="E67" s="107"/>
-      <c r="F67" s="107"/>
-      <c r="G67" s="108"/>
-      <c r="H67" s="108"/>
-      <c r="I67" s="106"/>
-      <c r="J67" s="106"/>
-      <c r="K67" s="106"/>
-      <c r="L67" s="106"/>
-      <c r="M67" s="107"/>
+      <c r="A67" s="88"/>
+      <c r="B67" s="89"/>
+      <c r="C67" s="89"/>
+      <c r="D67" s="89"/>
+      <c r="E67" s="89"/>
+      <c r="F67" s="89"/>
+      <c r="G67" s="90"/>
+      <c r="H67" s="90"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="89"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="106"/>
-      <c r="B68" s="107"/>
-      <c r="C68" s="107"/>
-      <c r="D68" s="107"/>
-      <c r="E68" s="107"/>
-      <c r="F68" s="107"/>
-      <c r="G68" s="108"/>
-      <c r="H68" s="108"/>
-      <c r="I68" s="106"/>
-      <c r="J68" s="106"/>
-      <c r="K68" s="106"/>
-      <c r="L68" s="106"/>
-      <c r="M68" s="107"/>
+      <c r="A68" s="88"/>
+      <c r="B68" s="89"/>
+      <c r="C68" s="89"/>
+      <c r="D68" s="89"/>
+      <c r="E68" s="89"/>
+      <c r="F68" s="89"/>
+      <c r="G68" s="90"/>
+      <c r="H68" s="90"/>
+      <c r="I68" s="88"/>
+      <c r="J68" s="88"/>
+      <c r="K68" s="88"/>
+      <c r="L68" s="88"/>
+      <c r="M68" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:F29"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A21:A22"/>
@@ -6166,6 +6156,16 @@
     <mergeCell ref="I21:L21"/>
     <mergeCell ref="M21:M22"/>
     <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="E21:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit PM's documents and update project Plan
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20111009" sheetId="1" r:id="rId1"/>
@@ -12,19 +12,22 @@
     <sheet name="20111013" sheetId="3" r:id="rId3"/>
     <sheet name="20111020" sheetId="6" r:id="rId4"/>
     <sheet name="20111027" sheetId="8" r:id="rId5"/>
+    <sheet name="20111103" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20111020'!$B$20:$G$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20111027'!$B$21:$G$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'20111103'!$B$21:$G$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'20111020'!$A$1:$M$67</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'20111027'!$A$1:$M$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'20111103'!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="114">
   <si>
     <t>Task</t>
   </si>
@@ -355,6 +358,18 @@
   </si>
   <si>
     <t>Nghiên cứu Zend Form và thiết kế màn hình Global Configuration</t>
+  </si>
+  <si>
+    <t>ĐÁNH GIÁ CHẤT LƯỢNG LÀM VIỆC TUẦN 6</t>
+  </si>
+  <si>
+    <t>27/10/2011 - 03/11/2011</t>
+  </si>
+  <si>
+    <t>1. Review Screen Interface</t>
+  </si>
+  <si>
+    <t>28/10/2011</t>
   </si>
 </sst>
 </file>
@@ -807,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1042,6 +1057,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1095,6 +1113,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,39 +1446,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="101"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94" t="s">
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="99"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1461,13 +1491,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="94"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="96" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1491,7 +1521,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="96"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1543,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="96"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1535,7 +1565,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="96"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1587,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1609,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1631,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1623,7 +1653,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1675,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="96"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1667,7 +1697,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="96"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1719,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="97"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1744,10 +1774,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="101"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1770,22 +1800,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94" t="s">
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -1793,9 +1823,9 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1808,7 +1838,7 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="94"/>
+      <c r="I4" s="95"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -1817,7 +1847,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="96" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1844,7 +1874,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="96"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1869,7 +1899,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="96"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1894,7 +1924,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="96"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1919,7 +1949,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1944,7 +1974,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1969,7 +1999,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1994,7 +2024,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2019,7 +2049,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="96"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2074,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="96"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2069,7 +2099,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="97"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2214,10 +2244,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="100"/>
+      <c r="E1" s="101"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2240,22 +2270,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94" t="s">
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -2263,9 +2293,9 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2278,7 +2308,7 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="94"/>
+      <c r="I4" s="95"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -2287,7 +2317,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="96" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2314,7 +2344,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="96"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2339,7 +2369,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="96"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2394,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="96"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2389,7 +2419,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2414,7 +2444,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2439,7 +2469,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2464,7 +2494,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2491,7 +2521,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="96"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2516,7 +2546,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="96"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2543,7 +2573,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="97"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2672,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="E21" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2688,38 +2718,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
@@ -3127,43 +3157,43 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="101" t="s">
+      <c r="B20" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="106"/>
-      <c r="G20" s="101" t="s">
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="101" t="s">
+      <c r="H20" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="101" t="s">
+      <c r="I20" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="101"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="101" t="s">
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="110"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
       <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
@@ -3176,7 +3206,7 @@
       <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="101"/>
+      <c r="M21" s="102"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
@@ -4632,8 +4662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -4648,38 +4678,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
@@ -5104,49 +5134,49 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="101" t="s">
+      <c r="G21" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="101" t="s">
+      <c r="H21" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="I21" s="101" t="s">
+      <c r="I21" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="101"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101" t="s">
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
       <c r="I22" s="44" t="s">
         <v>34</v>
       </c>
@@ -5159,7 +5189,7 @@
       <c r="L22" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="101"/>
+      <c r="M22" s="102"/>
     </row>
     <row r="23" spans="1:13" s="62" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
@@ -5311,43 +5341,43 @@
       <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="101" t="s">
+      <c r="A28" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C28" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="105"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="101" t="s">
+      <c r="D28" s="106"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="101" t="s">
+      <c r="H28" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="101" t="s">
+      <c r="I28" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="101" t="s">
+      <c r="J28" s="102"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="24" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
-      <c r="B29" s="101"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="109"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
       <c r="I29" s="44" t="s">
         <v>34</v>
       </c>
@@ -5360,7 +5390,7 @@
       <c r="L29" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="101"/>
+      <c r="M29" s="102"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="49">
@@ -6147,6 +6177,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A21:A22"/>
@@ -6158,6 +6196,1533 @@
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="C21:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M68"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E39:E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="30" style="45" customWidth="1"/>
+    <col min="3" max="3" width="20" style="45" customWidth="1"/>
+    <col min="4" max="6" width="19.5703125" style="45" customWidth="1"/>
+    <col min="7" max="12" width="12.140625" style="45" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="45" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+    </row>
+    <row r="5" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="49">
+        <v>1</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="F6" s="51">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="52">
+        <f>AVERAGE(C6:F6)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="53">
+        <v>2</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="55">
+        <v>4</v>
+      </c>
+      <c r="E7" s="55">
+        <v>3</v>
+      </c>
+      <c r="F7" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="56">
+        <f t="shared" ref="G7:G16" si="0">AVERAGE(C7:F7)</f>
+        <v>3.5</v>
+      </c>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="53">
+        <v>3</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G8" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="53">
+        <v>4</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F9" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="53">
+        <v>5</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D10" s="55">
+        <v>4</v>
+      </c>
+      <c r="E10" s="55">
+        <v>3</v>
+      </c>
+      <c r="F10" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="53">
+        <v>6</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="53">
+        <v>7</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="55">
+        <v>4</v>
+      </c>
+      <c r="E12" s="55">
+        <v>3</v>
+      </c>
+      <c r="F12" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G12" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="53">
+        <v>8</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="55">
+        <v>4</v>
+      </c>
+      <c r="E13" s="55">
+        <v>3</v>
+      </c>
+      <c r="F13" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G13" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="53">
+        <v>9</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="53">
+        <v>10</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="53">
+        <v>11</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="56">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="102" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="64" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="102"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="102"/>
+    </row>
+    <row r="23" spans="1:13" s="62" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="65">
+        <v>1</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="68">
+        <v>40848</v>
+      </c>
+      <c r="E23" s="68">
+        <v>40848</v>
+      </c>
+      <c r="F23" s="63">
+        <v>9</v>
+      </c>
+      <c r="G23" s="72">
+        <v>9</v>
+      </c>
+      <c r="H23" s="72">
+        <v>3.75</v>
+      </c>
+      <c r="I23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="K23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="74">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="75"/>
+    </row>
+    <row r="24" spans="1:13" s="62" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A24" s="66">
+        <v>2</v>
+      </c>
+      <c r="B24" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="113">
+        <v>40848</v>
+      </c>
+      <c r="E24" s="113">
+        <v>40848</v>
+      </c>
+      <c r="F24" s="67">
+        <v>12</v>
+      </c>
+      <c r="G24" s="73">
+        <v>11</v>
+      </c>
+      <c r="H24" s="73">
+        <v>3.75</v>
+      </c>
+      <c r="I24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="J24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="K24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="L24" s="76">
+        <v>3.5</v>
+      </c>
+      <c r="M24" s="77"/>
+    </row>
+    <row r="25" spans="1:13" s="62" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="A25" s="78">
+        <v>3</v>
+      </c>
+      <c r="B25" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="114">
+        <v>40848</v>
+      </c>
+      <c r="E25" s="114">
+        <v>40848</v>
+      </c>
+      <c r="F25" s="79">
+        <v>15</v>
+      </c>
+      <c r="G25" s="82">
+        <v>15</v>
+      </c>
+      <c r="H25" s="82">
+        <v>3.25</v>
+      </c>
+      <c r="I25" s="83">
+        <v>3</v>
+      </c>
+      <c r="J25" s="83">
+        <v>3.5</v>
+      </c>
+      <c r="K25" s="83">
+        <v>4</v>
+      </c>
+      <c r="L25" s="83">
+        <v>3.5</v>
+      </c>
+      <c r="M25" s="84"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="85"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="86"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="89"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="106"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="102"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="A29" s="102"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="M29" s="102"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="49">
+        <v>1</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="37">
+        <v>40844</v>
+      </c>
+      <c r="H30" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="115">
+        <v>3.5</v>
+      </c>
+      <c r="J30" s="115">
+        <v>3.5</v>
+      </c>
+      <c r="K30" s="115">
+        <v>3.5</v>
+      </c>
+      <c r="L30" s="115">
+        <v>3.5</v>
+      </c>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="53">
+        <v>2</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H31" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J31" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K31" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L31" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="53">
+        <v>3</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H32" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J32" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K32" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L32" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="53">
+        <v>4</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H33" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J33" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K33" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L33" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="53">
+        <v>5</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H34" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J34" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K34" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L34" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="53">
+        <v>6</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H35" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J35" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K35" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L35" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="53">
+        <v>7</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H36" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I36" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J36" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K36" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L36" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="53">
+        <v>8</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H37" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J37" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K37" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L37" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="53">
+        <v>9</v>
+      </c>
+      <c r="B38" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H38" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J38" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K38" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L38" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="53">
+        <v>10</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H39" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J39" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K39" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L39" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="53">
+        <v>11</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="38">
+        <v>40844</v>
+      </c>
+      <c r="H40" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I40" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="J40" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="K40" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="L40" s="116">
+        <v>3.5</v>
+      </c>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="20"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="20"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="20"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="13"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="13"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="13"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="13"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="88"/>
+      <c r="J51" s="88"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="88"/>
+      <c r="M51" s="89"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="88"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
+      <c r="K52" s="88"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="89"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="88"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="90"/>
+      <c r="I53" s="88"/>
+      <c r="J53" s="88"/>
+      <c r="K53" s="88"/>
+      <c r="L53" s="88"/>
+      <c r="M53" s="89"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="88"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="90"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="88"/>
+      <c r="K54" s="88"/>
+      <c r="L54" s="88"/>
+      <c r="M54" s="89"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="88"/>
+      <c r="B55" s="89"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="89"/>
+      <c r="G55" s="90"/>
+      <c r="H55" s="90"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="88"/>
+      <c r="M55" s="89"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="88"/>
+      <c r="B56" s="89"/>
+      <c r="C56" s="89"/>
+      <c r="D56" s="89"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="89"/>
+      <c r="G56" s="90"/>
+      <c r="H56" s="90"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="88"/>
+      <c r="M56" s="89"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="88"/>
+      <c r="B57" s="89"/>
+      <c r="C57" s="89"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="89"/>
+      <c r="G57" s="90"/>
+      <c r="H57" s="90"/>
+      <c r="I57" s="88"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="88"/>
+      <c r="M57" s="89"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="88"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="89"/>
+      <c r="G58" s="90"/>
+      <c r="H58" s="90"/>
+      <c r="I58" s="88"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="88"/>
+      <c r="L58" s="88"/>
+      <c r="M58" s="89"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="88"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="89"/>
+      <c r="F59" s="89"/>
+      <c r="G59" s="90"/>
+      <c r="H59" s="90"/>
+      <c r="I59" s="88"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="88"/>
+      <c r="M59" s="89"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="88"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="89"/>
+      <c r="D60" s="89"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="89"/>
+      <c r="G60" s="90"/>
+      <c r="H60" s="90"/>
+      <c r="I60" s="88"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="88"/>
+      <c r="L60" s="88"/>
+      <c r="M60" s="89"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="89"/>
+      <c r="D61" s="89"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="89"/>
+      <c r="G61" s="90"/>
+      <c r="H61" s="90"/>
+      <c r="I61" s="88"/>
+      <c r="J61" s="88"/>
+      <c r="K61" s="88"/>
+      <c r="L61" s="88"/>
+      <c r="M61" s="89"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="88"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="89"/>
+      <c r="D62" s="89"/>
+      <c r="E62" s="89"/>
+      <c r="F62" s="89"/>
+      <c r="G62" s="90"/>
+      <c r="H62" s="90"/>
+      <c r="I62" s="88"/>
+      <c r="J62" s="88"/>
+      <c r="K62" s="88"/>
+      <c r="L62" s="88"/>
+      <c r="M62" s="89"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="88"/>
+      <c r="B63" s="89"/>
+      <c r="C63" s="89"/>
+      <c r="D63" s="89"/>
+      <c r="E63" s="89"/>
+      <c r="F63" s="89"/>
+      <c r="G63" s="90"/>
+      <c r="H63" s="90"/>
+      <c r="I63" s="88"/>
+      <c r="J63" s="88"/>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
+      <c r="M63" s="89"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="88"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="90"/>
+      <c r="H64" s="90"/>
+      <c r="I64" s="88"/>
+      <c r="J64" s="88"/>
+      <c r="K64" s="88"/>
+      <c r="L64" s="88"/>
+      <c r="M64" s="89"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="88"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="89"/>
+      <c r="E65" s="89"/>
+      <c r="F65" s="89"/>
+      <c r="G65" s="90"/>
+      <c r="H65" s="90"/>
+      <c r="I65" s="88"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="88"/>
+      <c r="L65" s="88"/>
+      <c r="M65" s="89"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="88"/>
+      <c r="B66" s="89"/>
+      <c r="C66" s="89"/>
+      <c r="D66" s="89"/>
+      <c r="E66" s="89"/>
+      <c r="F66" s="89"/>
+      <c r="G66" s="90"/>
+      <c r="H66" s="90"/>
+      <c r="I66" s="88"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="88"/>
+      <c r="M66" s="89"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="88"/>
+      <c r="B67" s="89"/>
+      <c r="C67" s="89"/>
+      <c r="D67" s="89"/>
+      <c r="E67" s="89"/>
+      <c r="F67" s="89"/>
+      <c r="G67" s="90"/>
+      <c r="H67" s="90"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="89"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="88"/>
+      <c r="B68" s="89"/>
+      <c r="C68" s="89"/>
+      <c r="D68" s="89"/>
+      <c r="E68" s="89"/>
+      <c r="F68" s="89"/>
+      <c r="G68" s="90"/>
+      <c r="H68" s="90"/>
+      <c r="I68" s="88"/>
+      <c r="J68" s="88"/>
+      <c r="K68" s="88"/>
+      <c r="L68" s="88"/>
+      <c r="M68" s="89"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M21:M22"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:F29"/>
@@ -6165,7 +7730,16 @@
     <mergeCell ref="H28:H29"/>
     <mergeCell ref="I28:L28"/>
     <mergeCell ref="M28:M29"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tổng hợp đánh giá
</commit_message>
<xml_diff>
--- a/Document/Tracking/TongHopDanhGia.xlsx
+++ b/Document/Tracking/TongHopDanhGia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="13335" windowHeight="5130" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="13335" windowHeight="5070" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="20111009" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="6">'20111110'!$A$1:$M$81</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="167">
   <si>
     <t>Task</t>
   </si>
@@ -519,13 +520,19 @@
     <t>3.5</t>
   </si>
   <si>
-    <t xml:space="preserve">- </t>
-  </si>
-  <si>
     <t>Make a lab ( How to using Zend_DB )</t>
   </si>
   <si>
     <t>Chưa tới dealine nhưng đã hoàn thành</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>0611/2011</t>
+  </si>
+  <si>
+    <t>bỏ qua ActicleCopy, ActicleGlobalConfig,</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1706,7 +1713,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1726,7 +1732,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1741,7 +1746,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1768,25 +1772,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1809,10 +1796,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1839,19 +1822,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1866,10 +1842,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="52" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2255,39 +2243,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D1" s="192" t="s">
+      <c r="D1" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="192"/>
+      <c r="E1" s="181"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="190" t="s">
+      <c r="B3" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="186" t="s">
+      <c r="C3" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="186" t="s">
+      <c r="E3" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186" t="s">
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="191"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2300,13 +2288,13 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="186"/>
+      <c r="I4" s="175"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="187" t="s">
+      <c r="C5" s="176" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2330,7 +2318,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="188"/>
+      <c r="C6" s="177"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2352,7 +2340,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="177"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2374,7 +2362,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2396,7 +2384,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="177"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2418,7 +2406,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2440,7 +2428,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="188"/>
+      <c r="C11" s="177"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2462,7 +2450,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="177"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2484,7 +2472,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="188"/>
+      <c r="C13" s="177"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2506,7 +2494,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="188"/>
+      <c r="C14" s="177"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2528,7 +2516,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="189"/>
+      <c r="C15" s="178"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2583,10 +2571,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="192" t="s">
+      <c r="D1" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="192"/>
+      <c r="E1" s="181"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2609,22 +2597,22 @@
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="190" t="s">
+      <c r="B3" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="186" t="s">
+      <c r="C3" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="186" t="s">
+      <c r="E3" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186" t="s">
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -2632,9 +2620,9 @@
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="191"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2647,7 +2635,7 @@
       <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="186"/>
+      <c r="I4" s="175"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -2656,7 +2644,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="187" t="s">
+      <c r="C5" s="176" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2683,7 +2671,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="188"/>
+      <c r="C6" s="177"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2708,7 +2696,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="177"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -2733,7 +2721,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2758,7 +2746,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="177"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2783,7 +2771,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2808,7 +2796,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="188"/>
+      <c r="C11" s="177"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2833,7 +2821,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="177"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2858,7 +2846,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="188"/>
+      <c r="C13" s="177"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2883,7 +2871,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="188"/>
+      <c r="C14" s="177"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2908,7 +2896,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="189"/>
+      <c r="C15" s="178"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -3053,10 +3041,10 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="192" t="s">
+      <c r="D1" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="192"/>
+      <c r="E1" s="181"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -3079,22 +3067,22 @@
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="190" t="s">
+      <c r="B3" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="186" t="s">
+      <c r="C3" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="186" t="s">
+      <c r="E3" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186" t="s">
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="1"/>
@@ -3102,9 +3090,9 @@
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="191"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
@@ -3117,7 +3105,7 @@
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="186"/>
+      <c r="I4" s="175"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -3126,7 +3114,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="187" t="s">
+      <c r="C5" s="176" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3153,7 +3141,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="188"/>
+      <c r="C6" s="177"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
@@ -3178,7 +3166,7 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="177"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
@@ -3203,7 +3191,7 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3228,7 +3216,7 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="177"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
@@ -3253,7 +3241,7 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -3278,7 +3266,7 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="188"/>
+      <c r="C11" s="177"/>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
@@ -3303,7 +3291,7 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="177"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -3330,7 +3318,7 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="188"/>
+      <c r="C13" s="177"/>
       <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3343,7 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="188"/>
+      <c r="C14" s="177"/>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
@@ -3382,7 +3370,7 @@
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="189"/>
+      <c r="C15" s="178"/>
       <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
@@ -3527,38 +3515,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="194"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="194"/>
-      <c r="K2" s="194"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="194"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="195" t="s">
+      <c r="A3" s="184" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="I3" s="195"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
+      <c r="B3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
@@ -3966,43 +3954,43 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="193" t="s">
+      <c r="A20" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="193" t="s">
+      <c r="B20" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="196" t="s">
+      <c r="C20" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="197"/>
-      <c r="E20" s="197"/>
-      <c r="F20" s="198"/>
-      <c r="G20" s="193" t="s">
+      <c r="D20" s="186"/>
+      <c r="E20" s="186"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="193" t="s">
+      <c r="H20" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="193" t="s">
+      <c r="I20" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="193"/>
-      <c r="K20" s="193"/>
-      <c r="L20" s="193"/>
-      <c r="M20" s="193" t="s">
+      <c r="J20" s="182"/>
+      <c r="K20" s="182"/>
+      <c r="L20" s="182"/>
+      <c r="M20" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="193"/>
-      <c r="B21" s="193"/>
-      <c r="C21" s="199"/>
-      <c r="D21" s="200"/>
-      <c r="E21" s="200"/>
-      <c r="F21" s="201"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
+      <c r="A21" s="182"/>
+      <c r="B21" s="182"/>
+      <c r="C21" s="188"/>
+      <c r="D21" s="189"/>
+      <c r="E21" s="189"/>
+      <c r="F21" s="190"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="182"/>
       <c r="I21" s="8" t="s">
         <v>34</v>
       </c>
@@ -4015,7 +4003,7 @@
       <c r="L21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="193"/>
+      <c r="M21" s="182"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
@@ -5487,38 +5475,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="192" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
-      <c r="J3" s="203"/>
-      <c r="K3" s="203"/>
-      <c r="L3" s="203"/>
-      <c r="M3" s="203"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
@@ -5943,49 +5931,49 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="193" t="s">
+      <c r="A21" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="193" t="s">
+      <c r="B21" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="193" t="s">
+      <c r="C21" s="182" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="193" t="s">
+      <c r="D21" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="193" t="s">
+      <c r="E21" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="193" t="s">
+      <c r="F21" s="182" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="193" t="s">
+      <c r="G21" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="193" t="s">
+      <c r="H21" s="182" t="s">
         <v>89</v>
       </c>
-      <c r="I21" s="193" t="s">
+      <c r="I21" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
-      <c r="M21" s="193" t="s">
+      <c r="J21" s="182"/>
+      <c r="K21" s="182"/>
+      <c r="L21" s="182"/>
+      <c r="M21" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="193"/>
-      <c r="B22" s="193"/>
-      <c r="C22" s="193"/>
-      <c r="D22" s="193"/>
-      <c r="E22" s="193"/>
-      <c r="F22" s="193"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="193"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="182"/>
+      <c r="D22" s="182"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="182"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="182"/>
       <c r="I22" s="44" t="s">
         <v>34</v>
       </c>
@@ -5998,7 +5986,7 @@
       <c r="L22" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="193"/>
+      <c r="M22" s="182"/>
     </row>
     <row r="23" spans="1:13" s="62" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="65">
@@ -6150,43 +6138,43 @@
       <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="193" t="s">
+      <c r="A28" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="193" t="s">
+      <c r="B28" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="196" t="s">
+      <c r="C28" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="197"/>
-      <c r="E28" s="197"/>
-      <c r="F28" s="198"/>
-      <c r="G28" s="193" t="s">
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="187"/>
+      <c r="G28" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="193" t="s">
+      <c r="H28" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="193" t="s">
+      <c r="I28" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="193"/>
-      <c r="K28" s="193"/>
-      <c r="L28" s="193"/>
-      <c r="M28" s="193" t="s">
+      <c r="J28" s="182"/>
+      <c r="K28" s="182"/>
+      <c r="L28" s="182"/>
+      <c r="M28" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="193"/>
-      <c r="B29" s="193"/>
-      <c r="C29" s="199"/>
-      <c r="D29" s="200"/>
-      <c r="E29" s="200"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="193"/>
-      <c r="H29" s="193"/>
+      <c r="A29" s="182"/>
+      <c r="B29" s="182"/>
+      <c r="C29" s="188"/>
+      <c r="D29" s="189"/>
+      <c r="E29" s="189"/>
+      <c r="F29" s="190"/>
+      <c r="G29" s="182"/>
+      <c r="H29" s="182"/>
       <c r="I29" s="44" t="s">
         <v>34</v>
       </c>
@@ -6199,7 +6187,7 @@
       <c r="L29" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="193"/>
+      <c r="M29" s="182"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="49">
@@ -7031,38 +7019,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="191" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="192" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
-      <c r="J3" s="203"/>
-      <c r="K3" s="203"/>
-      <c r="L3" s="203"/>
-      <c r="M3" s="203"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
@@ -7487,49 +7475,49 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="193" t="s">
+      <c r="A21" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="193" t="s">
+      <c r="B21" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="193" t="s">
+      <c r="C21" s="182" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="193" t="s">
+      <c r="D21" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="193" t="s">
+      <c r="E21" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="193" t="s">
+      <c r="F21" s="182" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="193" t="s">
+      <c r="G21" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="193" t="s">
+      <c r="H21" s="182" t="s">
         <v>89</v>
       </c>
-      <c r="I21" s="193" t="s">
+      <c r="I21" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
-      <c r="M21" s="193" t="s">
+      <c r="J21" s="182"/>
+      <c r="K21" s="182"/>
+      <c r="L21" s="182"/>
+      <c r="M21" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="193"/>
-      <c r="B22" s="193"/>
-      <c r="C22" s="193"/>
-      <c r="D22" s="193"/>
-      <c r="E22" s="193"/>
-      <c r="F22" s="193"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="193"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="182"/>
+      <c r="D22" s="182"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="182"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="182"/>
       <c r="I22" s="94" t="s">
         <v>34</v>
       </c>
@@ -7542,7 +7530,7 @@
       <c r="L22" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="193"/>
+      <c r="M22" s="182"/>
     </row>
     <row r="23" spans="1:13" s="62" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="65">
@@ -7694,43 +7682,43 @@
       <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="193" t="s">
+      <c r="A28" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="193" t="s">
+      <c r="B28" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="196" t="s">
+      <c r="C28" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="197"/>
-      <c r="E28" s="197"/>
-      <c r="F28" s="198"/>
-      <c r="G28" s="193" t="s">
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="187"/>
+      <c r="G28" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="193" t="s">
+      <c r="H28" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="193" t="s">
+      <c r="I28" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="193"/>
-      <c r="K28" s="193"/>
-      <c r="L28" s="193"/>
-      <c r="M28" s="193" t="s">
+      <c r="J28" s="182"/>
+      <c r="K28" s="182"/>
+      <c r="L28" s="182"/>
+      <c r="M28" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="193"/>
-      <c r="B29" s="193"/>
-      <c r="C29" s="199"/>
-      <c r="D29" s="200"/>
-      <c r="E29" s="200"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="193"/>
-      <c r="H29" s="193"/>
+      <c r="A29" s="182"/>
+      <c r="B29" s="182"/>
+      <c r="C29" s="188"/>
+      <c r="D29" s="189"/>
+      <c r="E29" s="189"/>
+      <c r="F29" s="190"/>
+      <c r="G29" s="182"/>
+      <c r="H29" s="182"/>
       <c r="I29" s="94" t="s">
         <v>34</v>
       </c>
@@ -7743,7 +7731,7 @@
       <c r="L29" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="193"/>
+      <c r="M29" s="182"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="49">
@@ -8559,8 +8547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C19" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B19" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8577,38 +8565,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="191" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="192" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
-      <c r="J3" s="203"/>
-      <c r="K3" s="203"/>
-      <c r="L3" s="203"/>
-      <c r="M3" s="203"/>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
@@ -8737,121 +8725,121 @@
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
     </row>
-    <row r="9" spans="1:13" s="153" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="150">
-        <v>4</v>
-      </c>
-      <c r="B9" s="151" t="s">
+    <row r="9" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="140">
+        <v>4</v>
+      </c>
+      <c r="B9" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="152">
+      <c r="C9" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="142">
         <v>2.5</v>
       </c>
-      <c r="E9" s="152">
+      <c r="E9" s="142">
         <v>2.5</v>
       </c>
-      <c r="F9" s="152">
+      <c r="F9" s="142">
         <v>3.5</v>
       </c>
       <c r="G9" s="52">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
-      <c r="L9" s="154"/>
-      <c r="M9" s="154"/>
-    </row>
-    <row r="10" spans="1:13" s="168" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="165">
+      <c r="I9" s="144"/>
+      <c r="J9" s="144"/>
+      <c r="K9" s="144"/>
+      <c r="L9" s="144"/>
+      <c r="M9" s="144"/>
+    </row>
+    <row r="10" spans="1:13" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="153">
         <v>5</v>
       </c>
-      <c r="B10" s="166" t="s">
+      <c r="B10" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="167">
-        <v>2</v>
-      </c>
-      <c r="D10" s="167">
-        <v>2</v>
-      </c>
-      <c r="E10" s="167">
-        <v>3</v>
-      </c>
-      <c r="F10" s="167">
-        <v>3.5</v>
+      <c r="C10" s="155">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="155">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="155">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="155">
+        <v>3</v>
       </c>
       <c r="G10" s="52">
         <f t="shared" si="0"/>
         <v>2.625</v>
       </c>
-      <c r="I10" s="169"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="169"/>
-      <c r="M10" s="169"/>
-    </row>
-    <row r="11" spans="1:13" s="153" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="150">
+      <c r="I10" s="157"/>
+      <c r="J10" s="157"/>
+      <c r="K10" s="157"/>
+      <c r="L10" s="157"/>
+      <c r="M10" s="157"/>
+    </row>
+    <row r="11" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="140">
         <v>6</v>
       </c>
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="D11" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="E11" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="152">
+      <c r="C11" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="142">
         <v>3.5</v>
       </c>
       <c r="G11" s="52">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="154"/>
-      <c r="L11" s="154"/>
-      <c r="M11" s="154"/>
-    </row>
-    <row r="12" spans="1:13" s="153" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="150">
+      <c r="I11" s="144"/>
+      <c r="J11" s="144"/>
+      <c r="K11" s="144"/>
+      <c r="L11" s="144"/>
+      <c r="M11" s="144"/>
+    </row>
+    <row r="12" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="140">
         <v>7</v>
       </c>
-      <c r="B12" s="151" t="s">
+      <c r="B12" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="E12" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="152">
+      <c r="C12" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="E12" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="F12" s="142">
         <v>3.5</v>
       </c>
       <c r="G12" s="52">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="154"/>
+      <c r="I12" s="144"/>
+      <c r="J12" s="144"/>
+      <c r="K12" s="144"/>
+      <c r="L12" s="144"/>
+      <c r="M12" s="144"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="53">
@@ -8860,21 +8848,21 @@
       <c r="B13" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="55">
-        <v>3</v>
-      </c>
-      <c r="D13" s="55">
-        <v>3</v>
-      </c>
-      <c r="E13" s="55">
-        <v>3</v>
-      </c>
-      <c r="F13" s="55">
-        <v>3</v>
+      <c r="C13" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="F13" s="142">
+        <v>3.5</v>
       </c>
       <c r="G13" s="52">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I13" s="47"/>
       <c r="J13" s="47"/>
@@ -8889,21 +8877,21 @@
       <c r="B14" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="D14" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="E14" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="152">
-        <v>3.5</v>
+      <c r="C14" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="142">
+        <v>4</v>
       </c>
       <c r="G14" s="52">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.625</v>
       </c>
       <c r="I14" s="47"/>
       <c r="J14" s="47"/>
@@ -8928,11 +8916,11 @@
         <v>3</v>
       </c>
       <c r="F15" s="55">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G15" s="52">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.125</v>
       </c>
       <c r="I15" s="47"/>
       <c r="J15" s="47"/>
@@ -8947,21 +8935,21 @@
       <c r="B16" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="D16" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="E16" s="152">
-        <v>3.5</v>
-      </c>
-      <c r="F16" s="152">
+      <c r="C16" s="142">
+        <v>3.5</v>
+      </c>
+      <c r="D16" s="142">
+        <v>4</v>
+      </c>
+      <c r="E16" s="142">
+        <v>4</v>
+      </c>
+      <c r="F16" s="142">
         <v>3.5</v>
       </c>
       <c r="G16" s="52">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="I16" s="47"/>
       <c r="J16" s="47"/>
@@ -9031,43 +9019,43 @@
       <c r="M20" s="89"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="193" t="s">
+      <c r="A21" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="193" t="s">
+      <c r="B21" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="196" t="s">
+      <c r="C21" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="197"/>
-      <c r="E21" s="197"/>
-      <c r="F21" s="198"/>
-      <c r="G21" s="193" t="s">
+      <c r="D21" s="186"/>
+      <c r="E21" s="186"/>
+      <c r="F21" s="187"/>
+      <c r="G21" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="193" t="s">
+      <c r="H21" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="193" t="s">
+      <c r="I21" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
-      <c r="M21" s="193" t="s">
+      <c r="J21" s="182"/>
+      <c r="K21" s="182"/>
+      <c r="L21" s="182"/>
+      <c r="M21" s="182" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="193"/>
-      <c r="B22" s="193"/>
-      <c r="C22" s="199"/>
-      <c r="D22" s="200"/>
-      <c r="E22" s="200"/>
-      <c r="F22" s="201"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="193"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="188"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="190"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="182"/>
       <c r="I22" s="105" t="s">
         <v>34</v>
       </c>
@@ -9080,16 +9068,16 @@
       <c r="L22" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="193"/>
-    </row>
-    <row r="23" spans="1:13" s="114" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="M22" s="182"/>
+    </row>
+    <row r="23" spans="1:13" s="113" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="106">
         <v>1</v>
       </c>
-      <c r="B23" s="204" t="s">
+      <c r="B23" s="193" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="125" t="s">
+      <c r="C23" s="123" t="s">
         <v>128</v>
       </c>
       <c r="D23" s="108"/>
@@ -9098,59 +9086,59 @@
       <c r="G23" s="110">
         <v>40854</v>
       </c>
-      <c r="H23" s="145">
+      <c r="H23" s="110">
         <v>40854</v>
       </c>
-      <c r="I23" s="112">
-        <v>3</v>
-      </c>
-      <c r="J23" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="K23" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="L23" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="M23" s="113"/>
-    </row>
-    <row r="24" spans="1:13" s="124" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="116">
+      <c r="I23" s="111">
+        <v>3</v>
+      </c>
+      <c r="J23" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="K23" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="L23" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="M23" s="112"/>
+    </row>
+    <row r="24" spans="1:13" s="122" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="115">
         <v>2</v>
       </c>
-      <c r="B24" s="205"/>
-      <c r="C24" s="126" t="s">
+      <c r="B24" s="194"/>
+      <c r="C24" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="127"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="129">
+      <c r="D24" s="125"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="126"/>
+      <c r="G24" s="170">
         <v>40856</v>
       </c>
-      <c r="H24" s="129">
+      <c r="H24" s="170">
         <v>40856</v>
       </c>
-      <c r="I24" s="130">
-        <v>3</v>
-      </c>
-      <c r="J24" s="144">
+      <c r="I24" s="127">
+        <v>3</v>
+      </c>
+      <c r="J24" s="139">
         <v>2</v>
       </c>
-      <c r="K24" s="144">
+      <c r="K24" s="139">
         <v>2</v>
       </c>
-      <c r="L24" s="130" t="s">
+      <c r="L24" s="127" t="s">
         <v>161</v>
       </c>
-      <c r="M24" s="131"/>
-    </row>
-    <row r="25" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M24" s="128"/>
+    </row>
+    <row r="25" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="106">
         <v>3</v>
       </c>
-      <c r="B25" s="204" t="s">
+      <c r="B25" s="193" t="s">
         <v>126</v>
       </c>
       <c r="C25" s="107" t="s">
@@ -9159,41 +9147,41 @@
       <c r="D25" s="108"/>
       <c r="E25" s="108"/>
       <c r="F25" s="109"/>
-      <c r="G25" s="142">
+      <c r="G25" s="171">
         <v>40851</v>
       </c>
-      <c r="H25" s="146">
+      <c r="H25" s="171">
         <v>40852</v>
       </c>
-      <c r="I25" s="112">
+      <c r="I25" s="111">
         <v>2</v>
       </c>
-      <c r="J25" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="K25" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="L25" s="112">
+      <c r="J25" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="K25" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="L25" s="111">
         <v>2</v>
       </c>
-      <c r="M25" s="113"/>
+      <c r="M25" s="112"/>
     </row>
     <row r="26" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="115">
-        <v>4</v>
-      </c>
-      <c r="B26" s="206"/>
+      <c r="A26" s="114">
+        <v>4</v>
+      </c>
+      <c r="B26" s="195"/>
       <c r="C26" s="31" t="s">
         <v>132</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
       <c r="F26" s="33"/>
-      <c r="G26" s="143">
+      <c r="G26" s="172">
         <v>40852</v>
       </c>
-      <c r="H26" s="147">
+      <c r="H26" s="172">
         <v>40854</v>
       </c>
       <c r="I26" s="98">
@@ -9210,42 +9198,42 @@
       </c>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="116">
+    <row r="27" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="115">
         <v>5</v>
       </c>
-      <c r="B27" s="205"/>
-      <c r="C27" s="117" t="s">
+      <c r="B27" s="194"/>
+      <c r="C27" s="116" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="120">
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="119">
         <v>40855</v>
       </c>
-      <c r="H27" s="148">
+      <c r="H27" s="119">
         <v>40855</v>
       </c>
-      <c r="I27" s="122">
-        <v>3</v>
-      </c>
-      <c r="J27" s="122">
-        <v>3</v>
-      </c>
-      <c r="K27" s="122">
-        <v>3</v>
-      </c>
-      <c r="L27" s="122">
-        <v>3</v>
-      </c>
-      <c r="M27" s="123"/>
-    </row>
-    <row r="28" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="120">
+        <v>3</v>
+      </c>
+      <c r="J27" s="120">
+        <v>3</v>
+      </c>
+      <c r="K27" s="120">
+        <v>3</v>
+      </c>
+      <c r="L27" s="120">
+        <v>3</v>
+      </c>
+      <c r="M27" s="121"/>
+    </row>
+    <row r="28" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="106">
         <v>6</v>
       </c>
-      <c r="B28" s="204" t="s">
+      <c r="B28" s="193" t="s">
         <v>125</v>
       </c>
       <c r="C28" s="107" t="s">
@@ -9257,38 +9245,38 @@
       <c r="G28" s="110">
         <v>40851</v>
       </c>
-      <c r="H28" s="145">
+      <c r="H28" s="110">
         <v>40851</v>
       </c>
-      <c r="I28" s="112">
-        <v>3</v>
-      </c>
-      <c r="J28" s="112">
+      <c r="I28" s="111">
+        <v>3</v>
+      </c>
+      <c r="J28" s="111">
         <v>2</v>
       </c>
-      <c r="K28" s="112">
+      <c r="K28" s="111">
         <v>2</v>
       </c>
-      <c r="L28" s="112">
-        <v>3</v>
-      </c>
-      <c r="M28" s="113"/>
+      <c r="L28" s="111">
+        <v>3</v>
+      </c>
+      <c r="M28" s="112"/>
     </row>
     <row r="29" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="115">
+      <c r="A29" s="114">
         <v>7</v>
       </c>
-      <c r="B29" s="206"/>
+      <c r="B29" s="195"/>
       <c r="C29" s="31" t="s">
         <v>134</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="143">
+      <c r="G29" s="172">
         <v>40852</v>
       </c>
-      <c r="H29" s="147">
+      <c r="H29" s="172">
         <v>40853</v>
       </c>
       <c r="I29" s="98">
@@ -9305,189 +9293,189 @@
       </c>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116">
+    <row r="30" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="115">
         <v>8</v>
       </c>
-      <c r="B30" s="205"/>
-      <c r="C30" s="117" t="s">
+      <c r="B30" s="194"/>
+      <c r="C30" s="116" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="120">
+      <c r="D30" s="117"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="119">
         <v>40857</v>
       </c>
-      <c r="H30" s="149">
+      <c r="H30" s="152">
         <v>40856</v>
       </c>
-      <c r="I30" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J30" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K30" s="122">
-        <v>3</v>
-      </c>
-      <c r="L30" s="122" t="s">
+      <c r="I30" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="J30" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="K30" s="120">
+        <v>3</v>
+      </c>
+      <c r="L30" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="M30" s="123" t="s">
+      <c r="M30" s="121" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="151" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="145">
+        <v>9</v>
+      </c>
+      <c r="B31" s="193" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="146" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="166">
+        <v>40854</v>
+      </c>
+      <c r="H31" s="173">
+        <v>40854</v>
+      </c>
+      <c r="I31" s="149">
+        <v>3</v>
+      </c>
+      <c r="J31" s="149">
+        <v>2</v>
+      </c>
+      <c r="K31" s="149">
+        <v>2</v>
+      </c>
+      <c r="L31" s="149">
+        <v>3</v>
+      </c>
+      <c r="M31" s="150"/>
+    </row>
+    <row r="32" spans="1:13" s="122" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="129">
+        <v>10</v>
+      </c>
+      <c r="B32" s="194"/>
+      <c r="C32" s="130" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="119">
+        <v>40857</v>
+      </c>
+      <c r="H32" s="119">
+        <v>40857</v>
+      </c>
+      <c r="I32" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="J32" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="K32" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="L32" s="120" t="s">
+        <v>161</v>
+      </c>
+      <c r="M32" s="121"/>
+    </row>
+    <row r="33" spans="1:13" s="151" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="145">
+        <v>11</v>
+      </c>
+      <c r="B33" s="193" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="158" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="147"/>
+      <c r="E33" s="147"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="174">
+        <v>40853</v>
+      </c>
+      <c r="H33" s="149" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="163" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="155">
-        <v>9</v>
-      </c>
-      <c r="B31" s="204" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="156" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="159">
+      <c r="I33" s="149" t="s">
+        <v>164</v>
+      </c>
+      <c r="J33" s="149" t="s">
+        <v>164</v>
+      </c>
+      <c r="K33" s="149" t="s">
+        <v>164</v>
+      </c>
+      <c r="L33" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="M33" s="150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="164" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="159">
+        <v>12</v>
+      </c>
+      <c r="B34" s="195"/>
+      <c r="C34" s="160" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="161"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="162"/>
+      <c r="G34" s="174">
         <v>40854</v>
       </c>
-      <c r="H31" s="160">
-        <v>40854</v>
-      </c>
-      <c r="I31" s="161">
-        <v>3</v>
-      </c>
-      <c r="J31" s="161">
-        <v>2</v>
-      </c>
-      <c r="K31" s="161">
-        <v>2</v>
-      </c>
-      <c r="L31" s="161">
-        <v>3</v>
-      </c>
-      <c r="M31" s="162"/>
-    </row>
-    <row r="32" spans="1:13" s="124" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="132">
-        <v>10</v>
-      </c>
-      <c r="B32" s="205"/>
-      <c r="C32" s="133" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" s="118"/>
-      <c r="E32" s="118"/>
-      <c r="F32" s="119"/>
-      <c r="G32" s="120">
-        <v>40857</v>
-      </c>
-      <c r="H32" s="120">
-        <v>40857</v>
-      </c>
-      <c r="I32" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J32" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K32" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L32" s="122" t="s">
-        <v>161</v>
-      </c>
-      <c r="M32" s="123"/>
-    </row>
-    <row r="33" spans="1:13" s="163" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="155">
-        <v>11</v>
-      </c>
-      <c r="B33" s="204" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="170" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="157"/>
-      <c r="E33" s="157"/>
-      <c r="F33" s="158"/>
-      <c r="G33" s="159">
-        <v>40851</v>
-      </c>
-      <c r="H33" s="171" t="s">
-        <v>162</v>
-      </c>
-      <c r="I33" s="184" t="s">
-        <v>97</v>
-      </c>
-      <c r="J33" s="172" t="s">
-        <v>97</v>
-      </c>
-      <c r="K33" s="172" t="s">
-        <v>97</v>
-      </c>
-      <c r="L33" s="172" t="s">
-        <v>97</v>
-      </c>
-      <c r="M33" s="162" t="s">
+      <c r="H34" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="I34" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="J34" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="K34" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="L34" s="98">
+        <v>3.5</v>
+      </c>
+      <c r="M34" s="163" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="179" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="173">
-        <v>12</v>
-      </c>
-      <c r="B34" s="206"/>
-      <c r="C34" s="174" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="175"/>
-      <c r="E34" s="175"/>
-      <c r="F34" s="176"/>
-      <c r="G34" s="177">
-        <v>40854</v>
-      </c>
-      <c r="H34" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="I34" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="J34" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="K34" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="L34" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="M34" s="178" t="s">
-        <v>137</v>
-      </c>
-    </row>
     <row r="35" spans="1:13" s="89" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="115">
+      <c r="A35" s="114">
         <v>13</v>
       </c>
-      <c r="B35" s="206"/>
+      <c r="B35" s="195"/>
       <c r="C35" s="104" t="s">
         <v>139</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
       <c r="F35" s="33"/>
-      <c r="G35" s="38">
+      <c r="G35" s="93">
         <v>40855</v>
       </c>
       <c r="H35" s="93">
         <v>40855</v>
       </c>
-      <c r="I35" s="185">
+      <c r="I35" s="169">
         <v>3</v>
       </c>
       <c r="J35" s="98">
@@ -9497,160 +9485,160 @@
         <v>3</v>
       </c>
       <c r="L35" s="98">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M35" s="13"/>
     </row>
-    <row r="36" spans="1:13" s="124" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="116">
+    <row r="36" spans="1:13" s="122" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="115">
         <v>14</v>
       </c>
-      <c r="B36" s="205"/>
-      <c r="C36" s="135" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="118"/>
-      <c r="E36" s="118"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="120">
+      <c r="B36" s="194"/>
+      <c r="C36" s="132" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="117"/>
+      <c r="E36" s="117"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="119">
         <v>40857</v>
       </c>
-      <c r="H36" s="164">
+      <c r="H36" s="152">
         <v>40856</v>
       </c>
-      <c r="I36" s="122">
-        <v>4</v>
-      </c>
-      <c r="J36" s="122">
-        <v>4</v>
-      </c>
-      <c r="K36" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L36" s="122" t="s">
+      <c r="I36" s="120">
+        <v>4</v>
+      </c>
+      <c r="J36" s="120">
+        <v>4</v>
+      </c>
+      <c r="K36" s="120">
+        <v>4</v>
+      </c>
+      <c r="L36" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="M36" s="123"/>
-    </row>
-    <row r="37" spans="1:13" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="155">
+      <c r="M36" s="121"/>
+    </row>
+    <row r="37" spans="1:13" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="145">
         <v>15</v>
       </c>
-      <c r="B37" s="204" t="s">
+      <c r="B37" s="193" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="180" t="s">
+      <c r="C37" s="165" t="s">
         <v>140</v>
       </c>
-      <c r="D37" s="157"/>
-      <c r="E37" s="157"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="159">
+      <c r="D37" s="147"/>
+      <c r="E37" s="147"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="166">
         <v>40854</v>
       </c>
-      <c r="H37" s="181">
+      <c r="H37" s="166">
         <v>40854</v>
       </c>
-      <c r="I37" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="J37" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="K37" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="L37" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="M37" s="162"/>
-    </row>
-    <row r="38" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="132">
+      <c r="I37" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="J37" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="K37" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="L37" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="M37" s="150"/>
+    </row>
+    <row r="38" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="129">
         <v>16</v>
       </c>
-      <c r="B38" s="205"/>
-      <c r="C38" s="136" t="s">
+      <c r="B38" s="194"/>
+      <c r="C38" s="133" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="127"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="120">
+      <c r="D38" s="125"/>
+      <c r="E38" s="125"/>
+      <c r="F38" s="118"/>
+      <c r="G38" s="119">
         <v>40856</v>
       </c>
-      <c r="H38" s="121">
+      <c r="H38" s="119">
         <v>40856</v>
       </c>
-      <c r="I38" s="122">
-        <v>3</v>
-      </c>
-      <c r="J38" s="122">
-        <v>3</v>
-      </c>
-      <c r="K38" s="122">
-        <v>3</v>
-      </c>
-      <c r="L38" s="122">
-        <v>3</v>
-      </c>
-      <c r="M38" s="123"/>
-    </row>
-    <row r="39" spans="1:13" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="155">
+      <c r="I38" s="120">
+        <v>3</v>
+      </c>
+      <c r="J38" s="120">
+        <v>3</v>
+      </c>
+      <c r="K38" s="120">
+        <v>3</v>
+      </c>
+      <c r="L38" s="120">
+        <v>3</v>
+      </c>
+      <c r="M38" s="121"/>
+    </row>
+    <row r="39" spans="1:13" s="151" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="145">
         <v>17</v>
       </c>
-      <c r="B39" s="204" t="s">
+      <c r="B39" s="193" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="180" t="s">
+      <c r="C39" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="157"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="158"/>
-      <c r="G39" s="159">
+      <c r="D39" s="147"/>
+      <c r="E39" s="147"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="166">
         <v>40851</v>
       </c>
-      <c r="H39" s="181">
+      <c r="H39" s="166">
         <v>40851</v>
       </c>
-      <c r="I39" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="J39" s="161">
-        <v>3</v>
-      </c>
-      <c r="K39" s="161">
-        <v>3</v>
-      </c>
-      <c r="L39" s="161">
-        <v>3.5</v>
-      </c>
-      <c r="M39" s="162"/>
+      <c r="I39" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="J39" s="149">
+        <v>3</v>
+      </c>
+      <c r="K39" s="149">
+        <v>3</v>
+      </c>
+      <c r="L39" s="149">
+        <v>3.5</v>
+      </c>
+      <c r="M39" s="150"/>
     </row>
     <row r="40" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="134">
+      <c r="A40" s="131">
         <v>18</v>
       </c>
-      <c r="B40" s="206"/>
+      <c r="B40" s="195"/>
       <c r="C40" s="31" t="s">
         <v>143</v>
       </c>
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
       <c r="F40" s="33"/>
-      <c r="G40" s="38">
+      <c r="G40" s="93">
         <v>40854</v>
       </c>
-      <c r="H40" s="93">
-        <v>40854</v>
+      <c r="H40" s="93" t="s">
+        <v>165</v>
       </c>
       <c r="I40" s="98">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="J40" s="98">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K40" s="98">
         <v>4</v>
@@ -9660,44 +9648,44 @@
       </c>
       <c r="M40" s="13"/>
     </row>
-    <row r="41" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="132">
+    <row r="41" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="129">
         <v>19</v>
       </c>
-      <c r="B41" s="205"/>
-      <c r="C41" s="117" t="s">
+      <c r="B41" s="194"/>
+      <c r="C41" s="116" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="119"/>
-      <c r="G41" s="120">
+      <c r="D41" s="117"/>
+      <c r="E41" s="117"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="119">
         <v>40857</v>
       </c>
-      <c r="H41" s="182" t="s">
+      <c r="H41" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="I41" s="182" t="s">
+      <c r="I41" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="J41" s="182" t="s">
+      <c r="J41" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="K41" s="182" t="s">
+      <c r="K41" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="L41" s="182" t="s">
+      <c r="L41" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="M41" s="123" t="s">
+      <c r="M41" s="121" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="106">
         <v>20</v>
       </c>
-      <c r="B42" s="204" t="s">
+      <c r="B42" s="193" t="s">
         <v>118</v>
       </c>
       <c r="C42" s="107" t="s">
@@ -9709,35 +9697,35 @@
       <c r="G42" s="110">
         <v>40851</v>
       </c>
-      <c r="H42" s="111">
+      <c r="H42" s="110">
         <v>40851</v>
       </c>
-      <c r="I42" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="J42" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="K42" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="L42" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="M42" s="113"/>
+      <c r="I42" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="J42" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="K42" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="L42" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="M42" s="112"/>
     </row>
     <row r="43" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="134">
+      <c r="A43" s="131">
         <v>21</v>
       </c>
-      <c r="B43" s="206"/>
+      <c r="B43" s="195"/>
       <c r="C43" s="31" t="s">
         <v>146</v>
       </c>
       <c r="D43" s="32"/>
       <c r="E43" s="32"/>
       <c r="F43" s="33"/>
-      <c r="G43" s="38">
+      <c r="G43" s="93">
         <v>40852</v>
       </c>
       <c r="H43" s="93">
@@ -9753,22 +9741,22 @@
         <v>3</v>
       </c>
       <c r="L43" s="98">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M43" s="13"/>
     </row>
     <row r="44" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="115">
+      <c r="A44" s="114">
         <v>22</v>
       </c>
-      <c r="B44" s="206"/>
+      <c r="B44" s="195"/>
       <c r="C44" s="31" t="s">
         <v>148</v>
       </c>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
       <c r="F44" s="33"/>
-      <c r="G44" s="38">
+      <c r="G44" s="93">
         <v>40854</v>
       </c>
       <c r="H44" s="93">
@@ -9784,46 +9772,46 @@
         <v>3</v>
       </c>
       <c r="L44" s="98">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="116">
+    <row r="45" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="115">
         <v>23</v>
       </c>
-      <c r="B45" s="205"/>
-      <c r="C45" s="117" t="s">
+      <c r="B45" s="194"/>
+      <c r="C45" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="120">
+      <c r="D45" s="117"/>
+      <c r="E45" s="117"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="119">
         <v>40856</v>
       </c>
-      <c r="H45" s="121">
+      <c r="H45" s="119">
         <v>40856</v>
       </c>
-      <c r="I45" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J45" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K45" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L45" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="M45" s="123"/>
-    </row>
-    <row r="46" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I45" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="J45" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="K45" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="L45" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="M45" s="121"/>
+    </row>
+    <row r="46" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="106">
         <v>24</v>
       </c>
-      <c r="B46" s="204" t="s">
+      <c r="B46" s="193" t="s">
         <v>119</v>
       </c>
       <c r="C46" s="107" t="s">
@@ -9835,35 +9823,35 @@
       <c r="G46" s="110">
         <v>40851</v>
       </c>
-      <c r="H46" s="111">
+      <c r="H46" s="110">
         <v>40851</v>
       </c>
-      <c r="I46" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="J46" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="K46" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="L46" s="112">
-        <v>3.5</v>
-      </c>
-      <c r="M46" s="113"/>
+      <c r="I46" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="J46" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="K46" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="L46" s="111">
+        <v>4</v>
+      </c>
+      <c r="M46" s="112"/>
     </row>
     <row r="47" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="115">
+      <c r="A47" s="114">
         <v>25</v>
       </c>
-      <c r="B47" s="206"/>
+      <c r="B47" s="195"/>
       <c r="C47" s="31" t="s">
         <v>151</v>
       </c>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
       <c r="F47" s="33"/>
-      <c r="G47" s="38">
+      <c r="G47" s="93">
         <v>40852</v>
       </c>
       <c r="H47" s="93">
@@ -9879,22 +9867,22 @@
         <v>3.5</v>
       </c>
       <c r="L47" s="98">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:13" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="137">
+      <c r="A48" s="134">
         <v>26</v>
       </c>
-      <c r="B48" s="206"/>
+      <c r="B48" s="195"/>
       <c r="C48" s="31" t="s">
         <v>152</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
       <c r="F48" s="33"/>
-      <c r="G48" s="38">
+      <c r="G48" s="93">
         <v>40854</v>
       </c>
       <c r="H48" s="93">
@@ -9910,46 +9898,46 @@
         <v>3</v>
       </c>
       <c r="L48" s="98">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M48" s="13"/>
     </row>
-    <row r="49" spans="1:13" s="124" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="138">
+    <row r="49" spans="1:13" s="122" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="135">
         <v>27</v>
       </c>
-      <c r="B49" s="205"/>
-      <c r="C49" s="117" t="s">
+      <c r="B49" s="194"/>
+      <c r="C49" s="116" t="s">
         <v>153</v>
       </c>
-      <c r="D49" s="118"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="119"/>
-      <c r="G49" s="120">
+      <c r="D49" s="117"/>
+      <c r="E49" s="117"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="119">
         <v>40856</v>
       </c>
-      <c r="H49" s="121">
+      <c r="H49" s="119">
         <v>40856</v>
       </c>
-      <c r="I49" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J49" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K49" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L49" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="M49" s="123"/>
-    </row>
-    <row r="50" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="J49" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="K49" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="L49" s="120">
+        <v>4</v>
+      </c>
+      <c r="M49" s="121"/>
+    </row>
+    <row r="50" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="106">
         <v>28</v>
       </c>
-      <c r="B50" s="204" t="s">
+      <c r="B50" s="193" t="s">
         <v>120</v>
       </c>
       <c r="C50" s="107" t="s">
@@ -9961,35 +9949,35 @@
       <c r="G50" s="110">
         <v>40851</v>
       </c>
-      <c r="H50" s="111">
+      <c r="H50" s="110">
         <v>40851</v>
       </c>
-      <c r="I50" s="112">
-        <v>3</v>
-      </c>
-      <c r="J50" s="112">
-        <v>3</v>
-      </c>
-      <c r="K50" s="112">
-        <v>3</v>
-      </c>
-      <c r="L50" s="112">
-        <v>3</v>
-      </c>
-      <c r="M50" s="113"/>
+      <c r="I50" s="111">
+        <v>3</v>
+      </c>
+      <c r="J50" s="111">
+        <v>3</v>
+      </c>
+      <c r="K50" s="111">
+        <v>3</v>
+      </c>
+      <c r="L50" s="111">
+        <v>3.5</v>
+      </c>
+      <c r="M50" s="112"/>
     </row>
     <row r="51" spans="1:13" s="89" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="137">
+      <c r="A51" s="134">
         <v>29</v>
       </c>
-      <c r="B51" s="206"/>
+      <c r="B51" s="195"/>
       <c r="C51" s="31" t="s">
         <v>155</v>
       </c>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
       <c r="F51" s="33"/>
-      <c r="G51" s="38">
+      <c r="G51" s="93">
         <v>40854</v>
       </c>
       <c r="H51" s="93">
@@ -10007,46 +9995,48 @@
       <c r="L51" s="98">
         <v>3.5</v>
       </c>
-      <c r="M51" s="13"/>
-    </row>
-    <row r="52" spans="1:13" s="124" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="138">
+      <c r="M51" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="122" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="135">
         <v>30</v>
       </c>
-      <c r="B52" s="205"/>
-      <c r="C52" s="117" t="s">
+      <c r="B52" s="194"/>
+      <c r="C52" s="116" t="s">
         <v>156</v>
       </c>
-      <c r="D52" s="118"/>
-      <c r="E52" s="118"/>
-      <c r="F52" s="119"/>
-      <c r="G52" s="120">
+      <c r="D52" s="117"/>
+      <c r="E52" s="117"/>
+      <c r="F52" s="118"/>
+      <c r="G52" s="119">
         <v>40857</v>
       </c>
-      <c r="H52" s="182" t="s">
+      <c r="H52" s="167" t="s">
         <v>97</v>
       </c>
-      <c r="I52" s="183" t="s">
+      <c r="I52" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="J52" s="183" t="s">
+      <c r="J52" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="K52" s="183" t="s">
+      <c r="K52" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="L52" s="183" t="s">
+      <c r="L52" s="168" t="s">
         <v>97</v>
       </c>
-      <c r="M52" s="123" t="s">
+      <c r="M52" s="121" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="114" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="106">
         <v>31</v>
       </c>
-      <c r="B53" s="204" t="s">
+      <c r="B53" s="193" t="s">
         <v>121</v>
       </c>
       <c r="C53" s="107" t="s">
@@ -10058,129 +10048,129 @@
       <c r="G53" s="110">
         <v>40851</v>
       </c>
-      <c r="H53" s="111">
+      <c r="H53" s="110">
         <v>40851</v>
       </c>
-      <c r="I53" s="112">
-        <v>3</v>
-      </c>
-      <c r="J53" s="112">
-        <v>3</v>
-      </c>
-      <c r="K53" s="112">
-        <v>3</v>
-      </c>
-      <c r="L53" s="112">
-        <v>3</v>
-      </c>
-      <c r="M53" s="113"/>
-    </row>
-    <row r="54" spans="1:13" s="89" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="137">
+      <c r="I53" s="111">
+        <v>3</v>
+      </c>
+      <c r="J53" s="111">
+        <v>3</v>
+      </c>
+      <c r="K53" s="111">
+        <v>3</v>
+      </c>
+      <c r="L53" s="98">
+        <v>3.5</v>
+      </c>
+      <c r="M53" s="112"/>
+    </row>
+    <row r="54" spans="1:13" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="134">
         <v>32</v>
       </c>
-      <c r="B54" s="206"/>
+      <c r="B54" s="195"/>
       <c r="C54" s="31" t="s">
         <v>158</v>
       </c>
       <c r="D54" s="32"/>
       <c r="E54" s="32"/>
       <c r="F54" s="33"/>
-      <c r="G54" s="38">
+      <c r="G54" s="93">
         <v>40852</v>
       </c>
-      <c r="H54" s="38">
+      <c r="H54" s="93">
         <v>40852</v>
       </c>
-      <c r="I54" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J54" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K54" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L54" s="122">
+      <c r="I54" s="98">
+        <v>3</v>
+      </c>
+      <c r="J54" s="98">
+        <v>4</v>
+      </c>
+      <c r="K54" s="98">
+        <v>4</v>
+      </c>
+      <c r="L54" s="98">
         <v>3.5</v>
       </c>
       <c r="M54" s="13"/>
     </row>
-    <row r="55" spans="1:13" s="89" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="134">
+    <row r="55" spans="1:13" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="131">
         <v>33</v>
       </c>
-      <c r="B55" s="206"/>
+      <c r="B55" s="195"/>
       <c r="C55" s="31" t="s">
         <v>159</v>
       </c>
       <c r="D55" s="32"/>
       <c r="E55" s="32"/>
       <c r="F55" s="33"/>
-      <c r="G55" s="38">
+      <c r="G55" s="93">
         <v>40855</v>
       </c>
-      <c r="H55" s="38">
+      <c r="H55" s="93">
         <v>40855</v>
       </c>
-      <c r="I55" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J55" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K55" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L55" s="122">
+      <c r="I55" s="98">
+        <v>3</v>
+      </c>
+      <c r="J55" s="98">
+        <v>4</v>
+      </c>
+      <c r="K55" s="98">
+        <v>4</v>
+      </c>
+      <c r="L55" s="98">
         <v>3.5</v>
       </c>
       <c r="M55" s="13"/>
     </row>
-    <row r="56" spans="1:13" s="124" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="132">
+    <row r="56" spans="1:13" s="122" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="129">
         <v>34</v>
       </c>
-      <c r="B56" s="205"/>
-      <c r="C56" s="117" t="s">
+      <c r="B56" s="194"/>
+      <c r="C56" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="D56" s="118"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="119"/>
-      <c r="G56" s="120">
+      <c r="D56" s="117"/>
+      <c r="E56" s="117"/>
+      <c r="F56" s="118"/>
+      <c r="G56" s="119">
         <v>40857</v>
       </c>
-      <c r="H56" s="120">
+      <c r="H56" s="152">
         <v>40856</v>
       </c>
-      <c r="I56" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="J56" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="K56" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="L56" s="122">
-        <v>3.5</v>
-      </c>
-      <c r="M56" s="123"/>
+      <c r="I56" s="120">
+        <v>4</v>
+      </c>
+      <c r="J56" s="120">
+        <v>4</v>
+      </c>
+      <c r="K56" s="120">
+        <v>4</v>
+      </c>
+      <c r="L56" s="120">
+        <v>3.5</v>
+      </c>
+      <c r="M56" s="121"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="139"/>
-      <c r="B57" s="140"/>
+      <c r="A57" s="136"/>
+      <c r="B57" s="137"/>
       <c r="C57" s="103"/>
       <c r="D57" s="99"/>
       <c r="E57" s="99"/>
       <c r="F57" s="100"/>
       <c r="G57" s="101"/>
       <c r="H57" s="101"/>
-      <c r="I57" s="141"/>
-      <c r="J57" s="141"/>
-      <c r="K57" s="141"/>
-      <c r="L57" s="141"/>
+      <c r="I57" s="138"/>
+      <c r="J57" s="138"/>
+      <c r="K57" s="138"/>
+      <c r="L57" s="138"/>
       <c r="M57" s="102"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>